<commit_message>
Update OS version and R214001.
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSTASK/MS-OXWSTASK_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSTASK/MS-OXWSTASK_RequirementSpecification.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1959" uniqueCount="644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1960" uniqueCount="645">
   <si>
     <t>Req ID</t>
   </si>
@@ -2692,6 +2692,9 @@
   </si>
   <si>
     <t>[In t:TaskType Complex Type] ChangeCount: Specifies an integer value that specifies the number of times the task has changed since it was created.</t>
+  </si>
+  <si>
+    <t>6.0</t>
   </si>
 </sst>
 </file>
@@ -3019,9 +3022,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3044,30 +3044,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3102,145 +3078,38 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="43">
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
+  <dxfs count="31">
     <dxf>
       <font>
         <b val="0"/>
@@ -3560,6 +3429,80 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3689,34 +3632,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I290" tableType="xml" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I290" tableType="xml" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" connectionId="1">
   <autoFilter ref="A19:I290"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="40">
+    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="39">
+    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="38">
+    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="37">
+    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="36">
+    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="35">
+    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="34">
+    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="33">
+    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="7">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="32">
+    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="6">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -3725,12 +3668,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowBorderDxfId="31" tableBorderDxfId="30" totalsRowBorderDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="28"/>
-    <tableColumn id="2" name="Test" dataDxfId="27"/>
-    <tableColumn id="3" name="Description" dataDxfId="26"/>
+    <tableColumn id="1" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4026,8 +3969,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C123" sqref="C123"/>
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -4076,33 +4019,33 @@
       <c r="B3" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="35">
-        <v>6</v>
+      <c r="C3" s="63" t="s">
+        <v>644</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="36">
+      <c r="F3" s="35">
         <v>42261</v>
       </c>
-      <c r="G3" s="37"/>
+      <c r="G3" s="36"/>
       <c r="H3" s="4"/>
       <c r="I3" s="32"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" ht="21">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
       <c r="I4" s="32"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -4114,13 +4057,13 @@
       <c r="B5" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="48"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="58"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
@@ -4128,16 +4071,16 @@
       <c r="A6" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="48"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="58"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
@@ -4145,16 +4088,16 @@
       <c r="A7" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="52"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="62"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
@@ -4162,16 +4105,16 @@
       <c r="A8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="51"/>
-      <c r="I8" s="52"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="62"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
@@ -4179,16 +4122,16 @@
       <c r="A9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="58"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="49"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
     </row>
@@ -4196,33 +4139,33 @@
       <c r="A10" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="58"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="49"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="59" t="s">
+      <c r="B11" s="50" t="s">
         <v>559</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="55"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="46"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
     </row>
@@ -4233,7 +4176,7 @@
       <c r="B12" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="40" t="s">
         <v>1</v>
       </c>
       <c r="D12" s="29"/>
@@ -4241,7 +4184,7 @@
       <c r="F12" s="29"/>
       <c r="G12" s="29"/>
       <c r="H12" s="29"/>
-      <c r="I12" s="38"/>
+      <c r="I12" s="37"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
     </row>
@@ -4252,7 +4195,7 @@
       <c r="B13" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="42" t="s">
+      <c r="C13" s="41" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="30"/>
@@ -4260,7 +4203,7 @@
       <c r="F13" s="30"/>
       <c r="G13" s="30"/>
       <c r="H13" s="30"/>
-      <c r="I13" s="39"/>
+      <c r="I13" s="38"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
     </row>
@@ -4271,7 +4214,7 @@
       <c r="B14" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="41" t="s">
         <v>36</v>
       </c>
       <c r="D14" s="30"/>
@@ -4279,7 +4222,7 @@
       <c r="F14" s="30"/>
       <c r="G14" s="30"/>
       <c r="H14" s="30"/>
-      <c r="I14" s="39"/>
+      <c r="I14" s="38"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
     </row>
@@ -4290,7 +4233,7 @@
       <c r="B15" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="41" t="s">
         <v>31</v>
       </c>
       <c r="D15" s="31"/>
@@ -4298,24 +4241,24 @@
       <c r="F15" s="31"/>
       <c r="G15" s="31"/>
       <c r="H15" s="31"/>
-      <c r="I15" s="40"/>
+      <c r="I15" s="39"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
     </row>
     <row r="16" spans="1:11" ht="30" customHeight="1">
-      <c r="A16" s="44" t="s">
+      <c r="A16" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="61" t="s">
+      <c r="B16" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="62"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="54"/>
-      <c r="I16" s="55"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="46"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
     </row>
@@ -4323,16 +4266,16 @@
       <c r="A17" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="63" t="s">
+      <c r="B17" s="54" t="s">
         <v>561</v>
       </c>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="55"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="46"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
     </row>
@@ -4340,16 +4283,16 @@
       <c r="A18" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="53" t="s">
+      <c r="B18" s="44" t="s">
         <v>560</v>
       </c>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="54"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="55"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="46"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="M18" s="4"/>
@@ -5678,13 +5621,13 @@
         <v>19</v>
       </c>
       <c r="F71" s="25" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G71" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H71" s="25" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I71" s="27"/>
     </row>
@@ -11199,68 +11142,68 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B8:I8"/>
     <mergeCell ref="B18:I18"/>
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="B16:I16"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B8:I8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A20:H52 A35:I290">
-    <cfRule type="expression" dxfId="13" priority="53">
+    <cfRule type="expression" dxfId="30" priority="53">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="54">
+    <cfRule type="expression" dxfId="29" priority="54">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="61">
+    <cfRule type="expression" dxfId="28" priority="61">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:H52 A35:I290">
-    <cfRule type="expression" dxfId="10" priority="7">
+    <cfRule type="expression" dxfId="27" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="8">
+    <cfRule type="expression" dxfId="26" priority="8">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="25" priority="9">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F290">
-    <cfRule type="expression" dxfId="7" priority="13">
+    <cfRule type="expression" dxfId="24" priority="13">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="14">
+    <cfRule type="expression" dxfId="23" priority="14">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:I52">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="22" priority="4">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="21" priority="5">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="20" priority="6">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:I52">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="19" priority="1">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="18" priority="2">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="17" priority="3">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11298,21 +11241,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -11361,16 +11289,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11384,16 +11328,15 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update RS for TDI blocked
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSTASK/MS-OXWSTASK_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSTASK/MS-OXWSTASK_RequirementSpecification.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\E16 EWS update\20160310_Task\Docs\MS-OXWSTASK\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
   </bookViews>
@@ -2705,14 +2710,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="165" formatCode="0.0.0"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="177" formatCode="0.0.0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2955,7 +2960,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2989,7 +2994,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3025,8 +3030,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3110,113 +3115,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
+  <dxfs count="31">
     <dxf>
       <font>
         <b val="0"/>
@@ -3536,6 +3437,80 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3665,34 +3640,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I290" tableType="xml" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I290" tableType="xml" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" connectionId="1">
   <autoFilter ref="A19:I290"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="34">
+    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="33">
+    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="32">
+    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="31">
+    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="30">
+    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="29">
+    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="28">
+    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="27">
+    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="7">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="26">
+    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="6">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -3701,19 +3676,19 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowBorderDxfId="25" tableBorderDxfId="24" totalsRowBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="22"/>
-    <tableColumn id="2" name="Test" dataDxfId="21"/>
-    <tableColumn id="3" name="Description" dataDxfId="20"/>
+    <tableColumn id="1" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3755,7 +3730,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3790,7 +3765,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4002,26 +3977,24 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C119" sqref="C119"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="25.375" style="10" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.375" style="3" customWidth="1"/>
     <col min="8" max="8" width="14" style="3" customWidth="1"/>
-    <col min="9" max="9" width="28.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="28.75" style="3" customWidth="1"/>
     <col min="10" max="10" width="9" style="3" customWidth="1"/>
     <col min="11" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>555</v>
       </c>
@@ -4033,7 +4006,7 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>556</v>
       </c>
@@ -4047,7 +4020,7 @@
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="33"/>
       <c r="B3" s="34" t="s">
         <v>25</v>
@@ -4068,7 +4041,7 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:11" ht="21">
+    <row r="4" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="45" t="s">
         <v>24</v>
       </c>
@@ -4083,7 +4056,7 @@
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>13</v>
       </c>
@@ -4100,7 +4073,7 @@
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>0</v>
       </c>
@@ -4117,7 +4090,7 @@
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>38</v>
       </c>
@@ -4134,7 +4107,7 @@
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>1</v>
       </c>
@@ -4151,7 +4124,7 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" ht="78.75" customHeight="1">
+    <row r="9" spans="1:11" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>12</v>
       </c>
@@ -4168,7 +4141,7 @@
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="1:11" ht="33.75" customHeight="1">
+    <row r="10" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>2</v>
       </c>
@@ -4185,7 +4158,7 @@
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1">
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="42" t="s">
         <v>8</v>
       </c>
@@ -4202,7 +4175,7 @@
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>8</v>
       </c>
@@ -4221,7 +4194,7 @@
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>6</v>
       </c>
@@ -4240,7 +4213,7 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
         <v>7</v>
       </c>
@@ -4259,7 +4232,7 @@
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
         <v>3</v>
       </c>
@@ -4278,7 +4251,7 @@
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="1:11" ht="30" customHeight="1">
+    <row r="16" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="43" t="s">
         <v>23</v>
       </c>
@@ -4295,7 +4268,7 @@
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="1:13" ht="64.5" customHeight="1">
+    <row r="17" spans="1:13" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>4</v>
       </c>
@@ -4312,7 +4285,7 @@
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="1:13" ht="30" customHeight="1">
+    <row r="18" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>5</v>
       </c>
@@ -4330,7 +4303,7 @@
       <c r="K18" s="4"/>
       <c r="M18" s="4"/>
     </row>
-    <row r="19" spans="1:13" ht="30">
+    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>0</v>
       </c>
@@ -4360,7 +4333,7 @@
       </c>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:13" s="19" customFormat="1" ht="60">
+    <row r="20" spans="1:13" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.15">
       <c r="A20" s="18" t="s">
         <v>41</v>
       </c>
@@ -4385,7 +4358,7 @@
       </c>
       <c r="I20" s="20"/>
     </row>
-    <row r="21" spans="1:13" s="19" customFormat="1" ht="45">
+    <row r="21" spans="1:13" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A21" s="18" t="s">
         <v>42</v>
       </c>
@@ -4410,7 +4383,7 @@
       </c>
       <c r="I21" s="20"/>
     </row>
-    <row r="22" spans="1:13" s="19" customFormat="1" ht="30">
+    <row r="22" spans="1:13" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A22" s="18" t="s">
         <v>43</v>
       </c>
@@ -4435,7 +4408,7 @@
       </c>
       <c r="I22" s="20"/>
     </row>
-    <row r="23" spans="1:13" s="19" customFormat="1" ht="30">
+    <row r="23" spans="1:13" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A23" s="18" t="s">
         <v>44</v>
       </c>
@@ -4460,7 +4433,7 @@
       </c>
       <c r="I23" s="20"/>
     </row>
-    <row r="24" spans="1:13" s="19" customFormat="1" ht="30">
+    <row r="24" spans="1:13" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A24" s="18" t="s">
         <v>45</v>
       </c>
@@ -4485,7 +4458,7 @@
       </c>
       <c r="I24" s="20"/>
     </row>
-    <row r="25" spans="1:13" s="19" customFormat="1" ht="30">
+    <row r="25" spans="1:13" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A25" s="18" t="s">
         <v>46</v>
       </c>
@@ -4510,7 +4483,7 @@
       </c>
       <c r="I25" s="20"/>
     </row>
-    <row r="26" spans="1:13" s="19" customFormat="1" ht="45">
+    <row r="26" spans="1:13" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.15">
       <c r="A26" s="18" t="s">
         <v>47</v>
       </c>
@@ -4535,7 +4508,7 @@
       </c>
       <c r="I26" s="20"/>
     </row>
-    <row r="27" spans="1:13" s="19" customFormat="1">
+    <row r="27" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A27" s="18" t="s">
         <v>48</v>
       </c>
@@ -4560,7 +4533,7 @@
       </c>
       <c r="I27" s="20"/>
     </row>
-    <row r="28" spans="1:13" s="19" customFormat="1" ht="30">
+    <row r="28" spans="1:13" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A28" s="18" t="s">
         <v>49</v>
       </c>
@@ -4585,7 +4558,7 @@
       </c>
       <c r="I28" s="20"/>
     </row>
-    <row r="29" spans="1:13" s="19" customFormat="1" ht="45">
+    <row r="29" spans="1:13" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A29" s="18" t="s">
         <v>50</v>
       </c>
@@ -4612,7 +4585,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="19" customFormat="1" ht="45">
+    <row r="30" spans="1:13" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A30" s="18" t="s">
         <v>561</v>
       </c>
@@ -4639,7 +4612,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="19" customFormat="1" ht="30">
+    <row r="31" spans="1:13" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A31" s="18" t="s">
         <v>51</v>
       </c>
@@ -4664,7 +4637,7 @@
       </c>
       <c r="I31" s="20"/>
     </row>
-    <row r="32" spans="1:13" s="19" customFormat="1" ht="30">
+    <row r="32" spans="1:13" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A32" s="18" t="s">
         <v>52</v>
       </c>
@@ -4689,7 +4662,7 @@
       </c>
       <c r="I32" s="20"/>
     </row>
-    <row r="33" spans="1:9" s="19" customFormat="1" ht="30">
+    <row r="33" spans="1:9" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A33" s="18" t="s">
         <v>53</v>
       </c>
@@ -4714,7 +4687,7 @@
       </c>
       <c r="I33" s="20"/>
     </row>
-    <row r="34" spans="1:9" s="19" customFormat="1" ht="45">
+    <row r="34" spans="1:9" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.15">
       <c r="A34" s="18" t="s">
         <v>54</v>
       </c>
@@ -4739,7 +4712,7 @@
       </c>
       <c r="I34" s="20"/>
     </row>
-    <row r="35" spans="1:9" ht="45">
+    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
         <v>55</v>
       </c>
@@ -4764,7 +4737,7 @@
       </c>
       <c r="I35" s="27"/>
     </row>
-    <row r="36" spans="1:9" ht="30">
+    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
         <v>56</v>
       </c>
@@ -4789,7 +4762,7 @@
       </c>
       <c r="I36" s="27"/>
     </row>
-    <row r="37" spans="1:9" ht="30">
+    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
         <v>57</v>
       </c>
@@ -4814,7 +4787,7 @@
       </c>
       <c r="I37" s="27"/>
     </row>
-    <row r="38" spans="1:9" ht="30">
+    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="25" t="s">
         <v>58</v>
       </c>
@@ -4839,7 +4812,7 @@
       </c>
       <c r="I38" s="27"/>
     </row>
-    <row r="39" spans="1:9" ht="30">
+    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="25" t="s">
         <v>59</v>
       </c>
@@ -4864,7 +4837,7 @@
       </c>
       <c r="I39" s="27"/>
     </row>
-    <row r="40" spans="1:9" ht="30">
+    <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
         <v>60</v>
       </c>
@@ -4889,7 +4862,7 @@
       </c>
       <c r="I40" s="27"/>
     </row>
-    <row r="41" spans="1:9" ht="30">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="25" t="s">
         <v>61</v>
       </c>
@@ -4914,7 +4887,7 @@
       </c>
       <c r="I41" s="27"/>
     </row>
-    <row r="42" spans="1:9" ht="30">
+    <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="25" t="s">
         <v>62</v>
       </c>
@@ -4939,7 +4912,7 @@
       </c>
       <c r="I42" s="27"/>
     </row>
-    <row r="43" spans="1:9" ht="75">
+    <row r="43" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
         <v>63</v>
       </c>
@@ -4964,7 +4937,7 @@
       </c>
       <c r="I43" s="27"/>
     </row>
-    <row r="44" spans="1:9" ht="30">
+    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="25" t="s">
         <v>64</v>
       </c>
@@ -4989,7 +4962,7 @@
       </c>
       <c r="I44" s="27"/>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
         <v>65</v>
       </c>
@@ -5014,7 +4987,7 @@
       </c>
       <c r="I45" s="27"/>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="25" t="s">
         <v>66</v>
       </c>
@@ -5039,7 +5012,7 @@
       </c>
       <c r="I46" s="27"/>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="25" t="s">
         <v>67</v>
       </c>
@@ -5064,7 +5037,7 @@
       </c>
       <c r="I47" s="27"/>
     </row>
-    <row r="48" spans="1:9" ht="30">
+    <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="25" t="s">
         <v>68</v>
       </c>
@@ -5089,7 +5062,7 @@
       </c>
       <c r="I48" s="27"/>
     </row>
-    <row r="49" spans="1:9" ht="30">
+    <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="25" t="s">
         <v>69</v>
       </c>
@@ -5114,7 +5087,7 @@
       </c>
       <c r="I49" s="27"/>
     </row>
-    <row r="50" spans="1:9" ht="30">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="25" t="s">
         <v>70</v>
       </c>
@@ -5139,7 +5112,7 @@
       </c>
       <c r="I50" s="27"/>
     </row>
-    <row r="51" spans="1:9" ht="30">
+    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="25" t="s">
         <v>71</v>
       </c>
@@ -5164,7 +5137,7 @@
       </c>
       <c r="I51" s="27"/>
     </row>
-    <row r="52" spans="1:9" ht="30">
+    <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="25" t="s">
         <v>72</v>
       </c>
@@ -5189,7 +5162,7 @@
       </c>
       <c r="I52" s="27"/>
     </row>
-    <row r="53" spans="1:9" ht="30">
+    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="25" t="s">
         <v>124</v>
       </c>
@@ -5214,7 +5187,7 @@
       </c>
       <c r="I53" s="27"/>
     </row>
-    <row r="54" spans="1:9" ht="135">
+    <row r="54" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A54" s="25" t="s">
         <v>125</v>
       </c>
@@ -5239,7 +5212,7 @@
       </c>
       <c r="I54" s="27"/>
     </row>
-    <row r="55" spans="1:9" ht="45">
+    <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="25" t="s">
         <v>126</v>
       </c>
@@ -5264,7 +5237,7 @@
       </c>
       <c r="I55" s="27"/>
     </row>
-    <row r="56" spans="1:9" ht="135">
+    <row r="56" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A56" s="25" t="s">
         <v>127</v>
       </c>
@@ -5289,7 +5262,7 @@
       </c>
       <c r="I56" s="27"/>
     </row>
-    <row r="57" spans="1:9" ht="30">
+    <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="25" t="s">
         <v>128</v>
       </c>
@@ -5314,7 +5287,7 @@
       </c>
       <c r="I57" s="27"/>
     </row>
-    <row r="58" spans="1:9" ht="150">
+    <row r="58" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A58" s="25" t="s">
         <v>129</v>
       </c>
@@ -5339,7 +5312,7 @@
       </c>
       <c r="I58" s="27"/>
     </row>
-    <row r="59" spans="1:9" ht="150">
+    <row r="59" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A59" s="25" t="s">
         <v>73</v>
       </c>
@@ -5364,7 +5337,7 @@
       </c>
       <c r="I59" s="27"/>
     </row>
-    <row r="60" spans="1:9" ht="45">
+    <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="25" t="s">
         <v>74</v>
       </c>
@@ -5389,7 +5362,7 @@
       </c>
       <c r="I60" s="27"/>
     </row>
-    <row r="61" spans="1:9" ht="30">
+    <row r="61" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="25" t="s">
         <v>75</v>
       </c>
@@ -5414,7 +5387,7 @@
       </c>
       <c r="I61" s="27"/>
     </row>
-    <row r="62" spans="1:9" ht="45">
+    <row r="62" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="25" t="s">
         <v>76</v>
       </c>
@@ -5439,7 +5412,7 @@
       </c>
       <c r="I62" s="27"/>
     </row>
-    <row r="63" spans="1:9" ht="30">
+    <row r="63" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="25" t="s">
         <v>77</v>
       </c>
@@ -5464,7 +5437,7 @@
       </c>
       <c r="I63" s="27"/>
     </row>
-    <row r="64" spans="1:9" ht="120">
+    <row r="64" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A64" s="25" t="s">
         <v>78</v>
       </c>
@@ -5485,11 +5458,11 @@
         <v>15</v>
       </c>
       <c r="H64" s="25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I64" s="27"/>
     </row>
-    <row r="65" spans="1:9" ht="30">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="25" t="s">
         <v>79</v>
       </c>
@@ -5514,7 +5487,7 @@
       </c>
       <c r="I65" s="27"/>
     </row>
-    <row r="66" spans="1:9" ht="409.5">
+    <row r="66" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A66" s="25" t="s">
         <v>80</v>
       </c>
@@ -5539,7 +5512,7 @@
       </c>
       <c r="I66" s="27"/>
     </row>
-    <row r="67" spans="1:9" ht="75">
+    <row r="67" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="25" t="s">
         <v>81</v>
       </c>
@@ -5564,7 +5537,7 @@
       </c>
       <c r="I67" s="27"/>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="25" t="s">
         <v>82</v>
       </c>
@@ -5589,7 +5562,7 @@
       </c>
       <c r="I68" s="27"/>
     </row>
-    <row r="69" spans="1:9" ht="30">
+    <row r="69" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="25" t="s">
         <v>83</v>
       </c>
@@ -5614,7 +5587,7 @@
       </c>
       <c r="I69" s="27"/>
     </row>
-    <row r="70" spans="1:9" ht="45">
+    <row r="70" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="25" t="s">
         <v>84</v>
       </c>
@@ -5639,7 +5612,7 @@
       </c>
       <c r="I70" s="27"/>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="25" t="s">
         <v>575</v>
       </c>
@@ -5664,7 +5637,7 @@
       </c>
       <c r="I71" s="27"/>
     </row>
-    <row r="72" spans="1:9" ht="30">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="25" t="s">
         <v>85</v>
       </c>
@@ -5689,7 +5662,7 @@
       </c>
       <c r="I72" s="27"/>
     </row>
-    <row r="73" spans="1:9" ht="30">
+    <row r="73" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="25" t="s">
         <v>86</v>
       </c>
@@ -5714,7 +5687,7 @@
       </c>
       <c r="I73" s="27"/>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="25" t="s">
         <v>87</v>
       </c>
@@ -5739,7 +5712,7 @@
       </c>
       <c r="I74" s="27"/>
     </row>
-    <row r="75" spans="1:9" ht="30">
+    <row r="75" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="25" t="s">
         <v>88</v>
       </c>
@@ -5764,7 +5737,7 @@
       </c>
       <c r="I75" s="27"/>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="25" t="s">
         <v>639</v>
       </c>
@@ -5785,11 +5758,11 @@
         <v>15</v>
       </c>
       <c r="H76" s="25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I76" s="27"/>
     </row>
-    <row r="77" spans="1:9" ht="30">
+    <row r="77" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="25" t="s">
         <v>89</v>
       </c>
@@ -5814,7 +5787,7 @@
       </c>
       <c r="I77" s="27"/>
     </row>
-    <row r="78" spans="1:9" ht="30">
+    <row r="78" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="25" t="s">
         <v>90</v>
       </c>
@@ -5839,7 +5812,7 @@
       </c>
       <c r="I78" s="27"/>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="25" t="s">
         <v>91</v>
       </c>
@@ -5864,7 +5837,7 @@
       </c>
       <c r="I79" s="27"/>
     </row>
-    <row r="80" spans="1:9" ht="30">
+    <row r="80" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="25" t="s">
         <v>92</v>
       </c>
@@ -5889,7 +5862,7 @@
       </c>
       <c r="I80" s="27"/>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="25" t="s">
         <v>93</v>
       </c>
@@ -5914,7 +5887,7 @@
       </c>
       <c r="I81" s="27"/>
     </row>
-    <row r="82" spans="1:9" ht="30">
+    <row r="82" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="25" t="s">
         <v>94</v>
       </c>
@@ -5939,7 +5912,7 @@
       </c>
       <c r="I82" s="27"/>
     </row>
-    <row r="83" spans="1:9" ht="45">
+    <row r="83" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A83" s="25" t="s">
         <v>95</v>
       </c>
@@ -5964,7 +5937,7 @@
       </c>
       <c r="I83" s="27"/>
     </row>
-    <row r="84" spans="1:9" ht="30">
+    <row r="84" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="25" t="s">
         <v>96</v>
       </c>
@@ -5989,7 +5962,7 @@
       </c>
       <c r="I84" s="27"/>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="25" t="s">
         <v>580</v>
       </c>
@@ -6014,7 +5987,7 @@
       </c>
       <c r="I85" s="27"/>
     </row>
-    <row r="86" spans="1:9" ht="30">
+    <row r="86" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="25" t="s">
         <v>97</v>
       </c>
@@ -6039,7 +6012,7 @@
       </c>
       <c r="I86" s="27"/>
     </row>
-    <row r="87" spans="1:9" ht="30">
+    <row r="87" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="25" t="s">
         <v>98</v>
       </c>
@@ -6064,7 +6037,7 @@
       </c>
       <c r="I87" s="27"/>
     </row>
-    <row r="88" spans="1:9" ht="30">
+    <row r="88" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="25" t="s">
         <v>99</v>
       </c>
@@ -6089,7 +6062,7 @@
       </c>
       <c r="I88" s="27"/>
     </row>
-    <row r="89" spans="1:9" ht="30">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="25" t="s">
         <v>583</v>
       </c>
@@ -6114,7 +6087,7 @@
       </c>
       <c r="I89" s="27"/>
     </row>
-    <row r="90" spans="1:9" ht="30">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="25" t="s">
         <v>100</v>
       </c>
@@ -6139,7 +6112,7 @@
       </c>
       <c r="I90" s="27"/>
     </row>
-    <row r="91" spans="1:9" ht="30">
+    <row r="91" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="25" t="s">
         <v>101</v>
       </c>
@@ -6164,7 +6137,7 @@
       </c>
       <c r="I91" s="27"/>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="25" t="s">
         <v>102</v>
       </c>
@@ -6191,7 +6164,7 @@
       </c>
       <c r="I92" s="27"/>
     </row>
-    <row r="93" spans="1:9" ht="30">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="25" t="s">
         <v>103</v>
       </c>
@@ -6218,7 +6191,7 @@
       </c>
       <c r="I93" s="27"/>
     </row>
-    <row r="94" spans="1:9">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="25" t="s">
         <v>586</v>
       </c>
@@ -6239,11 +6212,11 @@
         <v>15</v>
       </c>
       <c r="H94" s="25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I94" s="27"/>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="25" t="s">
         <v>104</v>
       </c>
@@ -6268,7 +6241,7 @@
       </c>
       <c r="I95" s="27"/>
     </row>
-    <row r="96" spans="1:9" ht="30">
+    <row r="96" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="25" t="s">
         <v>105</v>
       </c>
@@ -6289,11 +6262,11 @@
         <v>15</v>
       </c>
       <c r="H96" s="25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I96" s="27"/>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="25" t="s">
         <v>106</v>
       </c>
@@ -6320,7 +6293,7 @@
       </c>
       <c r="I97" s="27"/>
     </row>
-    <row r="98" spans="1:9" ht="30">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="25" t="s">
         <v>107</v>
       </c>
@@ -6347,7 +6320,7 @@
       </c>
       <c r="I98" s="27"/>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="25" t="s">
         <v>588</v>
       </c>
@@ -6368,11 +6341,11 @@
         <v>15</v>
       </c>
       <c r="H99" s="25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I99" s="27"/>
     </row>
-    <row r="100" spans="1:9" ht="30">
+    <row r="100" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="25" t="s">
         <v>108</v>
       </c>
@@ -6397,7 +6370,7 @@
       </c>
       <c r="I100" s="27"/>
     </row>
-    <row r="101" spans="1:9">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="25" t="s">
         <v>590</v>
       </c>
@@ -6422,7 +6395,7 @@
       </c>
       <c r="I101" s="27"/>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="25" t="s">
         <v>109</v>
       </c>
@@ -6447,7 +6420,7 @@
       </c>
       <c r="I102" s="27"/>
     </row>
-    <row r="103" spans="1:9" ht="30">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="25" t="s">
         <v>110</v>
       </c>
@@ -6472,7 +6445,7 @@
       </c>
       <c r="I103" s="27"/>
     </row>
-    <row r="104" spans="1:9" ht="30">
+    <row r="104" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="25" t="s">
         <v>111</v>
       </c>
@@ -6497,7 +6470,7 @@
       </c>
       <c r="I104" s="27"/>
     </row>
-    <row r="105" spans="1:9" ht="30">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="25" t="s">
         <v>592</v>
       </c>
@@ -6522,7 +6495,7 @@
       </c>
       <c r="I105" s="27"/>
     </row>
-    <row r="106" spans="1:9" ht="30">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="25" t="s">
         <v>112</v>
       </c>
@@ -6547,7 +6520,7 @@
       </c>
       <c r="I106" s="27"/>
     </row>
-    <row r="107" spans="1:9" ht="30">
+    <row r="107" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="25" t="s">
         <v>113</v>
       </c>
@@ -6572,7 +6545,7 @@
       </c>
       <c r="I107" s="27"/>
     </row>
-    <row r="108" spans="1:9" ht="30">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="25" t="s">
         <v>114</v>
       </c>
@@ -6597,7 +6570,7 @@
       </c>
       <c r="I108" s="27"/>
     </row>
-    <row r="109" spans="1:9" ht="30">
+    <row r="109" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="25" t="s">
         <v>115</v>
       </c>
@@ -6622,7 +6595,7 @@
       </c>
       <c r="I109" s="27"/>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="25" t="s">
         <v>116</v>
       </c>
@@ -6647,7 +6620,7 @@
       </c>
       <c r="I110" s="27"/>
     </row>
-    <row r="111" spans="1:9" ht="30">
+    <row r="111" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="25" t="s">
         <v>117</v>
       </c>
@@ -6672,7 +6645,7 @@
       </c>
       <c r="I111" s="27"/>
     </row>
-    <row r="112" spans="1:9" ht="30">
+    <row r="112" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" s="25" t="s">
         <v>118</v>
       </c>
@@ -6697,7 +6670,7 @@
       </c>
       <c r="I112" s="27"/>
     </row>
-    <row r="113" spans="1:9" ht="30">
+    <row r="113" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="25" t="s">
         <v>119</v>
       </c>
@@ -6722,7 +6695,7 @@
       </c>
       <c r="I113" s="27"/>
     </row>
-    <row r="114" spans="1:9">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="25" t="s">
         <v>120</v>
       </c>
@@ -6747,7 +6720,7 @@
       </c>
       <c r="I114" s="27"/>
     </row>
-    <row r="115" spans="1:9" ht="30">
+    <row r="115" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="25" t="s">
         <v>121</v>
       </c>
@@ -6772,7 +6745,7 @@
       </c>
       <c r="I115" s="27"/>
     </row>
-    <row r="116" spans="1:9">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="25" t="s">
         <v>596</v>
       </c>
@@ -6793,11 +6766,11 @@
         <v>15</v>
       </c>
       <c r="H116" s="25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I116" s="27"/>
     </row>
-    <row r="117" spans="1:9">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="25" t="s">
         <v>122</v>
       </c>
@@ -6822,7 +6795,7 @@
       </c>
       <c r="I117" s="27"/>
     </row>
-    <row r="118" spans="1:9" ht="30">
+    <row r="118" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="25" t="s">
         <v>123</v>
       </c>
@@ -6847,7 +6820,7 @@
       </c>
       <c r="I118" s="27"/>
     </row>
-    <row r="119" spans="1:9" ht="30">
+    <row r="119" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="25" t="s">
         <v>598</v>
       </c>
@@ -6872,7 +6845,7 @@
       </c>
       <c r="I119" s="27"/>
     </row>
-    <row r="120" spans="1:9" ht="30">
+    <row r="120" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A120" s="25" t="s">
         <v>604</v>
       </c>
@@ -6897,7 +6870,7 @@
       </c>
       <c r="I120" s="27"/>
     </row>
-    <row r="121" spans="1:9" ht="60">
+    <row r="121" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A121" s="25" t="s">
         <v>605</v>
       </c>
@@ -6922,7 +6895,7 @@
       </c>
       <c r="I121" s="27"/>
     </row>
-    <row r="122" spans="1:9" ht="30">
+    <row r="122" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" s="25" t="s">
         <v>130</v>
       </c>
@@ -6947,7 +6920,7 @@
       </c>
       <c r="I122" s="27"/>
     </row>
-    <row r="123" spans="1:9" ht="135">
+    <row r="123" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A123" s="25" t="s">
         <v>131</v>
       </c>
@@ -6972,7 +6945,7 @@
       </c>
       <c r="I123" s="27"/>
     </row>
-    <row r="124" spans="1:9" ht="30">
+    <row r="124" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" s="25" t="s">
         <v>132</v>
       </c>
@@ -6997,7 +6970,7 @@
       </c>
       <c r="I124" s="27"/>
     </row>
-    <row r="125" spans="1:9" ht="135">
+    <row r="125" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A125" s="25" t="s">
         <v>133</v>
       </c>
@@ -7022,7 +6995,7 @@
       </c>
       <c r="I125" s="27"/>
     </row>
-    <row r="126" spans="1:9" ht="45">
+    <row r="126" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A126" s="25" t="s">
         <v>134</v>
       </c>
@@ -7047,7 +7020,7 @@
       </c>
       <c r="I126" s="27"/>
     </row>
-    <row r="127" spans="1:9" ht="30">
+    <row r="127" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A127" s="25" t="s">
         <v>135</v>
       </c>
@@ -7072,7 +7045,7 @@
       </c>
       <c r="I127" s="27"/>
     </row>
-    <row r="128" spans="1:9">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="25" t="s">
         <v>136</v>
       </c>
@@ -7097,7 +7070,7 @@
       </c>
       <c r="I128" s="27"/>
     </row>
-    <row r="129" spans="1:9">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="25" t="s">
         <v>137</v>
       </c>
@@ -7122,7 +7095,7 @@
       </c>
       <c r="I129" s="27"/>
     </row>
-    <row r="130" spans="1:9">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="25" t="s">
         <v>138</v>
       </c>
@@ -7147,7 +7120,7 @@
       </c>
       <c r="I130" s="27"/>
     </row>
-    <row r="131" spans="1:9" ht="30">
+    <row r="131" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A131" s="25" t="s">
         <v>139</v>
       </c>
@@ -7172,7 +7145,7 @@
       </c>
       <c r="I131" s="27"/>
     </row>
-    <row r="132" spans="1:9" ht="45">
+    <row r="132" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="25" t="s">
         <v>140</v>
       </c>
@@ -7197,7 +7170,7 @@
       </c>
       <c r="I132" s="27"/>
     </row>
-    <row r="133" spans="1:9" ht="285">
+    <row r="133" spans="1:9" ht="270" x14ac:dyDescent="0.25">
       <c r="A133" s="25" t="s">
         <v>141</v>
       </c>
@@ -7222,7 +7195,7 @@
       </c>
       <c r="I133" s="27"/>
     </row>
-    <row r="134" spans="1:9" ht="45">
+    <row r="134" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="25" t="s">
         <v>142</v>
       </c>
@@ -7247,7 +7220,7 @@
       </c>
       <c r="I134" s="27"/>
     </row>
-    <row r="135" spans="1:9" ht="30">
+    <row r="135" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" s="25" t="s">
         <v>143</v>
       </c>
@@ -7272,7 +7245,7 @@
       </c>
       <c r="I135" s="27"/>
     </row>
-    <row r="136" spans="1:9" ht="30">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="25" t="s">
         <v>612</v>
       </c>
@@ -7297,7 +7270,7 @@
       </c>
       <c r="I136" s="27"/>
     </row>
-    <row r="137" spans="1:9" ht="30">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="25" t="s">
         <v>144</v>
       </c>
@@ -7322,7 +7295,7 @@
       </c>
       <c r="I137" s="27"/>
     </row>
-    <row r="138" spans="1:9">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="25" t="s">
         <v>145</v>
       </c>
@@ -7347,7 +7320,7 @@
       </c>
       <c r="I138" s="27"/>
     </row>
-    <row r="139" spans="1:9">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="25" t="s">
         <v>146</v>
       </c>
@@ -7372,7 +7345,7 @@
       </c>
       <c r="I139" s="27"/>
     </row>
-    <row r="140" spans="1:9" ht="30">
+    <row r="140" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A140" s="25" t="s">
         <v>147</v>
       </c>
@@ -7397,7 +7370,7 @@
       </c>
       <c r="I140" s="27"/>
     </row>
-    <row r="141" spans="1:9" ht="30">
+    <row r="141" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A141" s="25" t="s">
         <v>148</v>
       </c>
@@ -7422,7 +7395,7 @@
       </c>
       <c r="I141" s="27"/>
     </row>
-    <row r="142" spans="1:9" ht="30">
+    <row r="142" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A142" s="25" t="s">
         <v>615</v>
       </c>
@@ -7447,7 +7420,7 @@
       </c>
       <c r="I142" s="27"/>
     </row>
-    <row r="143" spans="1:9" ht="45">
+    <row r="143" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" s="25" t="s">
         <v>616</v>
       </c>
@@ -7472,7 +7445,7 @@
       </c>
       <c r="I143" s="27"/>
     </row>
-    <row r="144" spans="1:9" ht="255">
+    <row r="144" spans="1:9" ht="240" x14ac:dyDescent="0.25">
       <c r="A144" s="25" t="s">
         <v>149</v>
       </c>
@@ -7497,7 +7470,7 @@
       </c>
       <c r="I144" s="27"/>
     </row>
-    <row r="145" spans="1:9" ht="45">
+    <row r="145" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A145" s="25" t="s">
         <v>150</v>
       </c>
@@ -7522,7 +7495,7 @@
       </c>
       <c r="I145" s="27"/>
     </row>
-    <row r="146" spans="1:9">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="25" t="s">
         <v>151</v>
       </c>
@@ -7547,7 +7520,7 @@
       </c>
       <c r="I146" s="27"/>
     </row>
-    <row r="147" spans="1:9">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="25" t="s">
         <v>152</v>
       </c>
@@ -7572,7 +7545,7 @@
       </c>
       <c r="I147" s="27"/>
     </row>
-    <row r="148" spans="1:9">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="25" t="s">
         <v>153</v>
       </c>
@@ -7597,7 +7570,7 @@
       </c>
       <c r="I148" s="27"/>
     </row>
-    <row r="149" spans="1:9">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="25" t="s">
         <v>154</v>
       </c>
@@ -7622,7 +7595,7 @@
       </c>
       <c r="I149" s="27"/>
     </row>
-    <row r="150" spans="1:9" ht="30">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="25" t="s">
         <v>155</v>
       </c>
@@ -7647,7 +7620,7 @@
       </c>
       <c r="I150" s="27"/>
     </row>
-    <row r="151" spans="1:9" ht="30">
+    <row r="151" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A151" s="25" t="s">
         <v>156</v>
       </c>
@@ -7672,7 +7645,7 @@
       </c>
       <c r="I151" s="27"/>
     </row>
-    <row r="152" spans="1:9" ht="45">
+    <row r="152" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A152" s="25" t="s">
         <v>157</v>
       </c>
@@ -7697,7 +7670,7 @@
       </c>
       <c r="I152" s="27"/>
     </row>
-    <row r="153" spans="1:9" ht="30">
+    <row r="153" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A153" s="25" t="s">
         <v>158</v>
       </c>
@@ -7722,7 +7695,7 @@
       </c>
       <c r="I153" s="27"/>
     </row>
-    <row r="154" spans="1:9" ht="30">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" s="25" t="s">
         <v>159</v>
       </c>
@@ -7747,7 +7720,7 @@
       </c>
       <c r="I154" s="27"/>
     </row>
-    <row r="155" spans="1:9" ht="409.5">
+    <row r="155" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A155" s="25" t="s">
         <v>160</v>
       </c>
@@ -7772,7 +7745,7 @@
       </c>
       <c r="I155" s="27"/>
     </row>
-    <row r="156" spans="1:9" ht="75">
+    <row r="156" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A156" s="25" t="s">
         <v>161</v>
       </c>
@@ -7797,7 +7770,7 @@
       </c>
       <c r="I156" s="27"/>
     </row>
-    <row r="157" spans="1:9" ht="30">
+    <row r="157" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" s="25" t="s">
         <v>162</v>
       </c>
@@ -7822,7 +7795,7 @@
       </c>
       <c r="I157" s="27"/>
     </row>
-    <row r="158" spans="1:9" ht="30">
+    <row r="158" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" s="25" t="s">
         <v>163</v>
       </c>
@@ -7847,7 +7820,7 @@
       </c>
       <c r="I158" s="27"/>
     </row>
-    <row r="159" spans="1:9" ht="30">
+    <row r="159" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" s="25" t="s">
         <v>164</v>
       </c>
@@ -7872,7 +7845,7 @@
       </c>
       <c r="I159" s="27"/>
     </row>
-    <row r="160" spans="1:9" ht="30">
+    <row r="160" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A160" s="25" t="s">
         <v>165</v>
       </c>
@@ -7897,7 +7870,7 @@
       </c>
       <c r="I160" s="27"/>
     </row>
-    <row r="161" spans="1:9" ht="30">
+    <row r="161" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A161" s="25" t="s">
         <v>166</v>
       </c>
@@ -7922,7 +7895,7 @@
       </c>
       <c r="I161" s="27"/>
     </row>
-    <row r="162" spans="1:9" ht="30">
+    <row r="162" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" s="25" t="s">
         <v>167</v>
       </c>
@@ -7947,7 +7920,7 @@
       </c>
       <c r="I162" s="27"/>
     </row>
-    <row r="163" spans="1:9" ht="30">
+    <row r="163" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" s="25" t="s">
         <v>168</v>
       </c>
@@ -7972,7 +7945,7 @@
       </c>
       <c r="I163" s="27"/>
     </row>
-    <row r="164" spans="1:9" ht="30">
+    <row r="164" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="25" t="s">
         <v>169</v>
       </c>
@@ -7997,7 +7970,7 @@
       </c>
       <c r="I164" s="27"/>
     </row>
-    <row r="165" spans="1:9" ht="30">
+    <row r="165" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A165" s="25" t="s">
         <v>170</v>
       </c>
@@ -8022,7 +7995,7 @@
       </c>
       <c r="I165" s="27"/>
     </row>
-    <row r="166" spans="1:9" ht="30">
+    <row r="166" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" s="25" t="s">
         <v>171</v>
       </c>
@@ -8047,7 +8020,7 @@
       </c>
       <c r="I166" s="27"/>
     </row>
-    <row r="167" spans="1:9" ht="30">
+    <row r="167" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A167" s="25" t="s">
         <v>172</v>
       </c>
@@ -8072,7 +8045,7 @@
       </c>
       <c r="I167" s="27"/>
     </row>
-    <row r="168" spans="1:9" ht="30">
+    <row r="168" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A168" s="25" t="s">
         <v>173</v>
       </c>
@@ -8097,7 +8070,7 @@
       </c>
       <c r="I168" s="27"/>
     </row>
-    <row r="169" spans="1:9" ht="30">
+    <row r="169" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A169" s="25" t="s">
         <v>174</v>
       </c>
@@ -8122,7 +8095,7 @@
       </c>
       <c r="I169" s="27"/>
     </row>
-    <row r="170" spans="1:9" ht="30">
+    <row r="170" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A170" s="25" t="s">
         <v>175</v>
       </c>
@@ -8147,7 +8120,7 @@
       </c>
       <c r="I170" s="27"/>
     </row>
-    <row r="171" spans="1:9" ht="30">
+    <row r="171" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A171" s="25" t="s">
         <v>176</v>
       </c>
@@ -8172,7 +8145,7 @@
       </c>
       <c r="I171" s="27"/>
     </row>
-    <row r="172" spans="1:9" ht="30">
+    <row r="172" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A172" s="25" t="s">
         <v>177</v>
       </c>
@@ -8197,7 +8170,7 @@
       </c>
       <c r="I172" s="27"/>
     </row>
-    <row r="173" spans="1:9" ht="30">
+    <row r="173" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A173" s="25" t="s">
         <v>178</v>
       </c>
@@ -8222,7 +8195,7 @@
       </c>
       <c r="I173" s="27"/>
     </row>
-    <row r="174" spans="1:9" ht="30">
+    <row r="174" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A174" s="25" t="s">
         <v>179</v>
       </c>
@@ -8247,7 +8220,7 @@
       </c>
       <c r="I174" s="27"/>
     </row>
-    <row r="175" spans="1:9" ht="30">
+    <row r="175" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A175" s="25" t="s">
         <v>180</v>
       </c>
@@ -8272,7 +8245,7 @@
       </c>
       <c r="I175" s="27"/>
     </row>
-    <row r="176" spans="1:9" ht="30">
+    <row r="176" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A176" s="25" t="s">
         <v>181</v>
       </c>
@@ -8297,7 +8270,7 @@
       </c>
       <c r="I176" s="27"/>
     </row>
-    <row r="177" spans="1:9" ht="30">
+    <row r="177" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" s="25" t="s">
         <v>182</v>
       </c>
@@ -8322,7 +8295,7 @@
       </c>
       <c r="I177" s="27"/>
     </row>
-    <row r="178" spans="1:9" ht="30">
+    <row r="178" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A178" s="25" t="s">
         <v>183</v>
       </c>
@@ -8347,7 +8320,7 @@
       </c>
       <c r="I178" s="27"/>
     </row>
-    <row r="179" spans="1:9" ht="30">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" s="25" t="s">
         <v>184</v>
       </c>
@@ -8372,7 +8345,7 @@
       </c>
       <c r="I179" s="27"/>
     </row>
-    <row r="180" spans="1:9" ht="30">
+    <row r="180" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A180" s="25" t="s">
         <v>185</v>
       </c>
@@ -8397,7 +8370,7 @@
       </c>
       <c r="I180" s="27"/>
     </row>
-    <row r="181" spans="1:9" ht="45">
+    <row r="181" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A181" s="25" t="s">
         <v>186</v>
       </c>
@@ -8422,7 +8395,7 @@
       </c>
       <c r="I181" s="27"/>
     </row>
-    <row r="182" spans="1:9" ht="30">
+    <row r="182" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A182" s="25" t="s">
         <v>187</v>
       </c>
@@ -8447,7 +8420,7 @@
       </c>
       <c r="I182" s="27"/>
     </row>
-    <row r="183" spans="1:9" ht="30">
+    <row r="183" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A183" s="25" t="s">
         <v>188</v>
       </c>
@@ -8472,7 +8445,7 @@
       </c>
       <c r="I183" s="27"/>
     </row>
-    <row r="184" spans="1:9" ht="45">
+    <row r="184" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A184" s="25" t="s">
         <v>189</v>
       </c>
@@ -8497,7 +8470,7 @@
       </c>
       <c r="I184" s="27"/>
     </row>
-    <row r="185" spans="1:9" ht="30">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" s="25" t="s">
         <v>190</v>
       </c>
@@ -8522,7 +8495,7 @@
       </c>
       <c r="I185" s="27"/>
     </row>
-    <row r="186" spans="1:9" ht="30">
+    <row r="186" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A186" s="25" t="s">
         <v>191</v>
       </c>
@@ -8547,7 +8520,7 @@
       </c>
       <c r="I186" s="27"/>
     </row>
-    <row r="187" spans="1:9" ht="30">
+    <row r="187" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A187" s="25" t="s">
         <v>192</v>
       </c>
@@ -8572,7 +8545,7 @@
       </c>
       <c r="I187" s="27"/>
     </row>
-    <row r="188" spans="1:9" ht="30">
+    <row r="188" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A188" s="25" t="s">
         <v>193</v>
       </c>
@@ -8597,7 +8570,7 @@
       </c>
       <c r="I188" s="27"/>
     </row>
-    <row r="189" spans="1:9" ht="30">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" s="25" t="s">
         <v>194</v>
       </c>
@@ -8622,7 +8595,7 @@
       </c>
       <c r="I189" s="27"/>
     </row>
-    <row r="190" spans="1:9" ht="30">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" s="25" t="s">
         <v>195</v>
       </c>
@@ -8647,7 +8620,7 @@
       </c>
       <c r="I190" s="27"/>
     </row>
-    <row r="191" spans="1:9" ht="30">
+    <row r="191" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A191" s="25" t="s">
         <v>196</v>
       </c>
@@ -8672,7 +8645,7 @@
       </c>
       <c r="I191" s="27"/>
     </row>
-    <row r="192" spans="1:9" ht="75">
+    <row r="192" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A192" s="25" t="s">
         <v>197</v>
       </c>
@@ -8697,7 +8670,7 @@
       </c>
       <c r="I192" s="27"/>
     </row>
-    <row r="193" spans="1:9" ht="240">
+    <row r="193" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A193" s="25" t="s">
         <v>198</v>
       </c>
@@ -8722,7 +8695,7 @@
       </c>
       <c r="I193" s="27"/>
     </row>
-    <row r="194" spans="1:9" ht="30">
+    <row r="194" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A194" s="25" t="s">
         <v>199</v>
       </c>
@@ -8747,7 +8720,7 @@
       </c>
       <c r="I194" s="27"/>
     </row>
-    <row r="195" spans="1:9" ht="75">
+    <row r="195" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A195" s="25" t="s">
         <v>200</v>
       </c>
@@ -8772,7 +8745,7 @@
       </c>
       <c r="I195" s="27"/>
     </row>
-    <row r="196" spans="1:9" ht="45">
+    <row r="196" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A196" s="25" t="s">
         <v>201</v>
       </c>
@@ -8797,7 +8770,7 @@
       </c>
       <c r="I196" s="27"/>
     </row>
-    <row r="197" spans="1:9" ht="30">
+    <row r="197" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A197" s="25" t="s">
         <v>202</v>
       </c>
@@ -8822,7 +8795,7 @@
       </c>
       <c r="I197" s="27"/>
     </row>
-    <row r="198" spans="1:9" ht="30">
+    <row r="198" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A198" s="25" t="s">
         <v>203</v>
       </c>
@@ -8847,7 +8820,7 @@
       </c>
       <c r="I198" s="27"/>
     </row>
-    <row r="199" spans="1:9" ht="75">
+    <row r="199" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A199" s="25" t="s">
         <v>204</v>
       </c>
@@ -8872,7 +8845,7 @@
       </c>
       <c r="I199" s="27"/>
     </row>
-    <row r="200" spans="1:9" ht="255">
+    <row r="200" spans="1:9" ht="240" x14ac:dyDescent="0.25">
       <c r="A200" s="25" t="s">
         <v>205</v>
       </c>
@@ -8897,7 +8870,7 @@
       </c>
       <c r="I200" s="27"/>
     </row>
-    <row r="201" spans="1:9" ht="30">
+    <row r="201" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A201" s="25" t="s">
         <v>206</v>
       </c>
@@ -8922,7 +8895,7 @@
       </c>
       <c r="I201" s="27"/>
     </row>
-    <row r="202" spans="1:9" ht="75">
+    <row r="202" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A202" s="25" t="s">
         <v>207</v>
       </c>
@@ -8947,7 +8920,7 @@
       </c>
       <c r="I202" s="27"/>
     </row>
-    <row r="203" spans="1:9" ht="30">
+    <row r="203" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A203" s="25" t="s">
         <v>208</v>
       </c>
@@ -8972,7 +8945,7 @@
       </c>
       <c r="I203" s="27"/>
     </row>
-    <row r="204" spans="1:9" ht="30">
+    <row r="204" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A204" s="25" t="s">
         <v>209</v>
       </c>
@@ -8997,7 +8970,7 @@
       </c>
       <c r="I204" s="27"/>
     </row>
-    <row r="205" spans="1:9" ht="30">
+    <row r="205" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A205" s="25" t="s">
         <v>210</v>
       </c>
@@ -9022,7 +8995,7 @@
       </c>
       <c r="I205" s="27"/>
     </row>
-    <row r="206" spans="1:9" ht="75">
+    <row r="206" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A206" s="25" t="s">
         <v>211</v>
       </c>
@@ -9047,7 +9020,7 @@
       </c>
       <c r="I206" s="27"/>
     </row>
-    <row r="207" spans="1:9" ht="240">
+    <row r="207" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A207" s="25" t="s">
         <v>212</v>
       </c>
@@ -9072,7 +9045,7 @@
       </c>
       <c r="I207" s="27"/>
     </row>
-    <row r="208" spans="1:9" ht="30">
+    <row r="208" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A208" s="25" t="s">
         <v>213</v>
       </c>
@@ -9097,7 +9070,7 @@
       </c>
       <c r="I208" s="27"/>
     </row>
-    <row r="209" spans="1:9" ht="75">
+    <row r="209" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A209" s="25" t="s">
         <v>214</v>
       </c>
@@ -9122,7 +9095,7 @@
       </c>
       <c r="I209" s="27"/>
     </row>
-    <row r="210" spans="1:9" ht="30">
+    <row r="210" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A210" s="25" t="s">
         <v>215</v>
       </c>
@@ -9147,7 +9120,7 @@
       </c>
       <c r="I210" s="27"/>
     </row>
-    <row r="211" spans="1:9" ht="30">
+    <row r="211" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A211" s="25" t="s">
         <v>216</v>
       </c>
@@ -9172,7 +9145,7 @@
       </c>
       <c r="I211" s="27"/>
     </row>
-    <row r="212" spans="1:9" ht="30">
+    <row r="212" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A212" s="25" t="s">
         <v>217</v>
       </c>
@@ -9197,7 +9170,7 @@
       </c>
       <c r="I212" s="27"/>
     </row>
-    <row r="213" spans="1:9" ht="30">
+    <row r="213" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A213" s="25" t="s">
         <v>218</v>
       </c>
@@ -9222,7 +9195,7 @@
       </c>
       <c r="I213" s="27"/>
     </row>
-    <row r="214" spans="1:9" ht="165">
+    <row r="214" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A214" s="25" t="s">
         <v>219</v>
       </c>
@@ -9247,7 +9220,7 @@
       </c>
       <c r="I214" s="27"/>
     </row>
-    <row r="215" spans="1:9" ht="45">
+    <row r="215" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A215" s="25" t="s">
         <v>220</v>
       </c>
@@ -9272,7 +9245,7 @@
       </c>
       <c r="I215" s="27"/>
     </row>
-    <row r="216" spans="1:9" ht="45">
+    <row r="216" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A216" s="25" t="s">
         <v>221</v>
       </c>
@@ -9297,7 +9270,7 @@
       </c>
       <c r="I216" s="27"/>
     </row>
-    <row r="217" spans="1:9" ht="45">
+    <row r="217" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A217" s="25" t="s">
         <v>222</v>
       </c>
@@ -9322,7 +9295,7 @@
       </c>
       <c r="I217" s="27"/>
     </row>
-    <row r="218" spans="1:9" ht="30">
+    <row r="218" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A218" s="25" t="s">
         <v>223</v>
       </c>
@@ -9347,7 +9320,7 @@
       </c>
       <c r="I218" s="27"/>
     </row>
-    <row r="219" spans="1:9" ht="75">
+    <row r="219" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A219" s="25" t="s">
         <v>224</v>
       </c>
@@ -9372,7 +9345,7 @@
       </c>
       <c r="I219" s="27"/>
     </row>
-    <row r="220" spans="1:9" ht="240">
+    <row r="220" spans="1:9" ht="240" x14ac:dyDescent="0.25">
       <c r="A220" s="25" t="s">
         <v>225</v>
       </c>
@@ -9397,7 +9370,7 @@
       </c>
       <c r="I220" s="27"/>
     </row>
-    <row r="221" spans="1:9" ht="30">
+    <row r="221" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A221" s="25" t="s">
         <v>226</v>
       </c>
@@ -9422,7 +9395,7 @@
       </c>
       <c r="I221" s="27"/>
     </row>
-    <row r="222" spans="1:9" ht="90">
+    <row r="222" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A222" s="25" t="s">
         <v>227</v>
       </c>
@@ -9447,7 +9420,7 @@
       </c>
       <c r="I222" s="27"/>
     </row>
-    <row r="223" spans="1:9" ht="30">
+    <row r="223" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A223" s="25" t="s">
         <v>228</v>
       </c>
@@ -9472,7 +9445,7 @@
       </c>
       <c r="I223" s="27"/>
     </row>
-    <row r="224" spans="1:9" ht="45">
+    <row r="224" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A224" s="25" t="s">
         <v>229</v>
       </c>
@@ -9493,11 +9466,11 @@
         <v>15</v>
       </c>
       <c r="H224" s="25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I224" s="27"/>
     </row>
-    <row r="225" spans="1:9" ht="30">
+    <row r="225" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A225" s="25" t="s">
         <v>230</v>
       </c>
@@ -9522,7 +9495,7 @@
       </c>
       <c r="I225" s="27"/>
     </row>
-    <row r="226" spans="1:9" ht="75">
+    <row r="226" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A226" s="25" t="s">
         <v>231</v>
       </c>
@@ -9547,7 +9520,7 @@
       </c>
       <c r="I226" s="27"/>
     </row>
-    <row r="227" spans="1:9" ht="240">
+    <row r="227" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A227" s="25" t="s">
         <v>232</v>
       </c>
@@ -9572,7 +9545,7 @@
       </c>
       <c r="I227" s="27"/>
     </row>
-    <row r="228" spans="1:9" ht="30">
+    <row r="228" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A228" s="25" t="s">
         <v>233</v>
       </c>
@@ -9597,7 +9570,7 @@
       </c>
       <c r="I228" s="27"/>
     </row>
-    <row r="229" spans="1:9" ht="75">
+    <row r="229" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A229" s="25" t="s">
         <v>234</v>
       </c>
@@ -9622,7 +9595,7 @@
       </c>
       <c r="I229" s="27"/>
     </row>
-    <row r="230" spans="1:9" ht="30">
+    <row r="230" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A230" s="25" t="s">
         <v>235</v>
       </c>
@@ -9647,7 +9620,7 @@
       </c>
       <c r="I230" s="27"/>
     </row>
-    <row r="231" spans="1:9" ht="30">
+    <row r="231" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A231" s="25" t="s">
         <v>236</v>
       </c>
@@ -9672,7 +9645,7 @@
       </c>
       <c r="I231" s="27"/>
     </row>
-    <row r="232" spans="1:9" ht="30">
+    <row r="232" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A232" s="25" t="s">
         <v>237</v>
       </c>
@@ -9697,7 +9670,7 @@
       </c>
       <c r="I232" s="27"/>
     </row>
-    <row r="233" spans="1:9" ht="75">
+    <row r="233" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A233" s="25" t="s">
         <v>238</v>
       </c>
@@ -9722,7 +9695,7 @@
       </c>
       <c r="I233" s="27"/>
     </row>
-    <row r="234" spans="1:9" ht="255">
+    <row r="234" spans="1:9" ht="240" x14ac:dyDescent="0.25">
       <c r="A234" s="25" t="s">
         <v>239</v>
       </c>
@@ -9747,7 +9720,7 @@
       </c>
       <c r="I234" s="27"/>
     </row>
-    <row r="235" spans="1:9" ht="30">
+    <row r="235" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A235" s="25" t="s">
         <v>240</v>
       </c>
@@ -9772,7 +9745,7 @@
       </c>
       <c r="I235" s="27"/>
     </row>
-    <row r="236" spans="1:9" ht="30">
+    <row r="236" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A236" s="25" t="s">
         <v>241</v>
       </c>
@@ -9797,7 +9770,7 @@
       </c>
       <c r="I236" s="27"/>
     </row>
-    <row r="237" spans="1:9" ht="45">
+    <row r="237" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A237" s="25" t="s">
         <v>242</v>
       </c>
@@ -9822,7 +9795,7 @@
       </c>
       <c r="I237" s="27"/>
     </row>
-    <row r="238" spans="1:9" ht="30">
+    <row r="238" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A238" s="25" t="s">
         <v>243</v>
       </c>
@@ -9847,7 +9820,7 @@
       </c>
       <c r="I238" s="27"/>
     </row>
-    <row r="239" spans="1:9" ht="45">
+    <row r="239" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A239" s="25" t="s">
         <v>244</v>
       </c>
@@ -9876,7 +9849,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="240" spans="1:9" ht="45">
+    <row r="240" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A240" s="25" t="s">
         <v>563</v>
       </c>
@@ -9905,7 +9878,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="241" spans="1:9" ht="165">
+    <row r="241" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A241" s="25" t="s">
         <v>245</v>
       </c>
@@ -9930,7 +9903,7 @@
       </c>
       <c r="I241" s="27"/>
     </row>
-    <row r="242" spans="1:9" ht="225">
+    <row r="242" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A242" s="25" t="s">
         <v>246</v>
       </c>
@@ -9955,7 +9928,7 @@
       </c>
       <c r="I242" s="27"/>
     </row>
-    <row r="243" spans="1:9" ht="30">
+    <row r="243" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A243" s="25" t="s">
         <v>247</v>
       </c>
@@ -9980,7 +9953,7 @@
       </c>
       <c r="I243" s="27"/>
     </row>
-    <row r="244" spans="1:9" ht="30">
+    <row r="244" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A244" s="25" t="s">
         <v>248</v>
       </c>
@@ -10005,7 +9978,7 @@
       </c>
       <c r="I244" s="27"/>
     </row>
-    <row r="245" spans="1:9" ht="30">
+    <row r="245" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A245" s="25" t="s">
         <v>249</v>
       </c>
@@ -10030,7 +10003,7 @@
       </c>
       <c r="I245" s="27"/>
     </row>
-    <row r="246" spans="1:9" ht="30">
+    <row r="246" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A246" s="25" t="s">
         <v>250</v>
       </c>
@@ -10055,7 +10028,7 @@
       </c>
       <c r="I246" s="27"/>
     </row>
-    <row r="247" spans="1:9" ht="90">
+    <row r="247" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A247" s="25" t="s">
         <v>251</v>
       </c>
@@ -10080,7 +10053,7 @@
       </c>
       <c r="I247" s="27"/>
     </row>
-    <row r="248" spans="1:9" ht="60">
+    <row r="248" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A248" s="25" t="s">
         <v>252</v>
       </c>
@@ -10105,7 +10078,7 @@
       </c>
       <c r="I248" s="27"/>
     </row>
-    <row r="249" spans="1:9" ht="409.5">
+    <row r="249" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A249" s="25" t="s">
         <v>253</v>
       </c>
@@ -10130,7 +10103,7 @@
       </c>
       <c r="I249" s="27"/>
     </row>
-    <row r="250" spans="1:9" ht="225">
+    <row r="250" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A250" s="25" t="s">
         <v>254</v>
       </c>
@@ -10155,7 +10128,7 @@
       </c>
       <c r="I250" s="27"/>
     </row>
-    <row r="251" spans="1:9" ht="30">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A251" s="25" t="s">
         <v>255</v>
       </c>
@@ -10180,7 +10153,7 @@
       </c>
       <c r="I251" s="27"/>
     </row>
-    <row r="252" spans="1:9" ht="270">
+    <row r="252" spans="1:9" ht="270" x14ac:dyDescent="0.25">
       <c r="A252" s="25" t="s">
         <v>256</v>
       </c>
@@ -10205,7 +10178,7 @@
       </c>
       <c r="I252" s="27"/>
     </row>
-    <row r="253" spans="1:9" ht="30">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A253" s="25" t="s">
         <v>257</v>
       </c>
@@ -10230,7 +10203,7 @@
       </c>
       <c r="I253" s="27"/>
     </row>
-    <row r="254" spans="1:9" ht="30">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A254" s="25" t="s">
         <v>258</v>
       </c>
@@ -10255,7 +10228,7 @@
       </c>
       <c r="I254" s="27"/>
     </row>
-    <row r="255" spans="1:9" ht="150">
+    <row r="255" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A255" s="25" t="s">
         <v>259</v>
       </c>
@@ -10280,7 +10253,7 @@
       </c>
       <c r="I255" s="27"/>
     </row>
-    <row r="256" spans="1:9" ht="135">
+    <row r="256" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A256" s="25" t="s">
         <v>260</v>
       </c>
@@ -10305,7 +10278,7 @@
       </c>
       <c r="I256" s="27"/>
     </row>
-    <row r="257" spans="1:9" ht="225">
+    <row r="257" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A257" s="25" t="s">
         <v>261</v>
       </c>
@@ -10330,7 +10303,7 @@
       </c>
       <c r="I257" s="27"/>
     </row>
-    <row r="258" spans="1:9" ht="255">
+    <row r="258" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="A258" s="25" t="s">
         <v>262</v>
       </c>
@@ -10355,7 +10328,7 @@
       </c>
       <c r="I258" s="27"/>
     </row>
-    <row r="259" spans="1:9" ht="30">
+    <row r="259" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A259" s="25" t="s">
         <v>263</v>
       </c>
@@ -10380,7 +10353,7 @@
       </c>
       <c r="I259" s="27"/>
     </row>
-    <row r="260" spans="1:9" ht="30">
+    <row r="260" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A260" s="25" t="s">
         <v>264</v>
       </c>
@@ -10405,7 +10378,7 @@
       </c>
       <c r="I260" s="27"/>
     </row>
-    <row r="261" spans="1:9" ht="135">
+    <row r="261" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A261" s="25" t="s">
         <v>265</v>
       </c>
@@ -10430,7 +10403,7 @@
       </c>
       <c r="I261" s="27"/>
     </row>
-    <row r="262" spans="1:9" ht="225">
+    <row r="262" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A262" s="25" t="s">
         <v>266</v>
       </c>
@@ -10455,7 +10428,7 @@
       </c>
       <c r="I262" s="27"/>
     </row>
-    <row r="263" spans="1:9" ht="270">
+    <row r="263" spans="1:9" ht="270" x14ac:dyDescent="0.25">
       <c r="A263" s="25" t="s">
         <v>267</v>
       </c>
@@ -10480,7 +10453,7 @@
       </c>
       <c r="I263" s="27"/>
     </row>
-    <row r="264" spans="1:9" ht="30">
+    <row r="264" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A264" s="25" t="s">
         <v>268</v>
       </c>
@@ -10505,7 +10478,7 @@
       </c>
       <c r="I264" s="27"/>
     </row>
-    <row r="265" spans="1:9" ht="45">
+    <row r="265" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A265" s="25" t="s">
         <v>269</v>
       </c>
@@ -10530,7 +10503,7 @@
       </c>
       <c r="I265" s="27"/>
     </row>
-    <row r="266" spans="1:9" ht="30">
+    <row r="266" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A266" s="25" t="s">
         <v>270</v>
       </c>
@@ -10555,7 +10528,7 @@
       </c>
       <c r="I266" s="27"/>
     </row>
-    <row r="267" spans="1:9" ht="45">
+    <row r="267" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A267" s="25" t="s">
         <v>271</v>
       </c>
@@ -10580,7 +10553,7 @@
       </c>
       <c r="I267" s="27"/>
     </row>
-    <row r="268" spans="1:9" ht="315">
+    <row r="268" spans="1:9" ht="315" x14ac:dyDescent="0.25">
       <c r="A268" s="25" t="s">
         <v>272</v>
       </c>
@@ -10605,7 +10578,7 @@
       </c>
       <c r="I268" s="27"/>
     </row>
-    <row r="269" spans="1:9" ht="30">
+    <row r="269" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A269" s="25" t="s">
         <v>273</v>
       </c>
@@ -10630,7 +10603,7 @@
       </c>
       <c r="I269" s="27"/>
     </row>
-    <row r="270" spans="1:9" ht="45">
+    <row r="270" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A270" s="25" t="s">
         <v>274</v>
       </c>
@@ -10655,7 +10628,7 @@
       </c>
       <c r="I270" s="27"/>
     </row>
-    <row r="271" spans="1:9" ht="30">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A271" s="25" t="s">
         <v>275</v>
       </c>
@@ -10680,7 +10653,7 @@
       </c>
       <c r="I271" s="27"/>
     </row>
-    <row r="272" spans="1:9" ht="30">
+    <row r="272" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A272" s="25" t="s">
         <v>276</v>
       </c>
@@ -10705,7 +10678,7 @@
       </c>
       <c r="I272" s="27"/>
     </row>
-    <row r="273" spans="1:9" ht="45">
+    <row r="273" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A273" s="25" t="s">
         <v>277</v>
       </c>
@@ -10730,7 +10703,7 @@
       </c>
       <c r="I273" s="27"/>
     </row>
-    <row r="274" spans="1:9" ht="30">
+    <row r="274" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A274" s="25" t="s">
         <v>278</v>
       </c>
@@ -10755,7 +10728,7 @@
       </c>
       <c r="I274" s="27"/>
     </row>
-    <row r="275" spans="1:9" ht="30">
+    <row r="275" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A275" s="25" t="s">
         <v>279</v>
       </c>
@@ -10780,7 +10753,7 @@
       </c>
       <c r="I275" s="27"/>
     </row>
-    <row r="276" spans="1:9" ht="30">
+    <row r="276" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A276" s="25" t="s">
         <v>280</v>
       </c>
@@ -10805,7 +10778,7 @@
       </c>
       <c r="I276" s="27"/>
     </row>
-    <row r="277" spans="1:9" ht="30">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A277" s="25" t="s">
         <v>281</v>
       </c>
@@ -10830,7 +10803,7 @@
       </c>
       <c r="I277" s="27"/>
     </row>
-    <row r="278" spans="1:9" ht="285">
+    <row r="278" spans="1:9" ht="285" x14ac:dyDescent="0.25">
       <c r="A278" s="25" t="s">
         <v>282</v>
       </c>
@@ -10855,7 +10828,7 @@
       </c>
       <c r="I278" s="27"/>
     </row>
-    <row r="279" spans="1:9" ht="30">
+    <row r="279" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A279" s="25" t="s">
         <v>283</v>
       </c>
@@ -10880,7 +10853,7 @@
       </c>
       <c r="I279" s="27"/>
     </row>
-    <row r="280" spans="1:9" ht="45">
+    <row r="280" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A280" s="25" t="s">
         <v>284</v>
       </c>
@@ -10905,7 +10878,7 @@
       </c>
       <c r="I280" s="27"/>
     </row>
-    <row r="281" spans="1:9" ht="60">
+    <row r="281" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A281" s="25" t="s">
         <v>285</v>
       </c>
@@ -10932,7 +10905,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="282" spans="1:9" ht="255">
+    <row r="282" spans="1:9" ht="240" x14ac:dyDescent="0.25">
       <c r="A282" s="25" t="s">
         <v>286</v>
       </c>
@@ -10957,7 +10930,7 @@
       </c>
       <c r="I282" s="27"/>
     </row>
-    <row r="283" spans="1:9" ht="30">
+    <row r="283" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A283" s="25" t="s">
         <v>287</v>
       </c>
@@ -10982,7 +10955,7 @@
       </c>
       <c r="I283" s="27"/>
     </row>
-    <row r="284" spans="1:9" ht="45">
+    <row r="284" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A284" s="25" t="s">
         <v>288</v>
       </c>
@@ -11007,7 +10980,7 @@
       </c>
       <c r="I284" s="27"/>
     </row>
-    <row r="285" spans="1:9" ht="30">
+    <row r="285" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A285" s="25" t="s">
         <v>289</v>
       </c>
@@ -11032,7 +11005,7 @@
       </c>
       <c r="I285" s="27"/>
     </row>
-    <row r="286" spans="1:9" ht="45">
+    <row r="286" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A286" s="25" t="s">
         <v>290</v>
       </c>
@@ -11057,7 +11030,7 @@
       </c>
       <c r="I286" s="27"/>
     </row>
-    <row r="287" spans="1:9" ht="30">
+    <row r="287" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A287" s="25" t="s">
         <v>291</v>
       </c>
@@ -11082,7 +11055,7 @@
       </c>
       <c r="I287" s="27"/>
     </row>
-    <row r="288" spans="1:9" ht="45">
+    <row r="288" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A288" s="25" t="s">
         <v>292</v>
       </c>
@@ -11107,7 +11080,7 @@
       </c>
       <c r="I288" s="27"/>
     </row>
-    <row r="289" spans="1:9" ht="45">
+    <row r="289" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A289" s="25" t="s">
         <v>293</v>
       </c>
@@ -11136,7 +11109,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="290" spans="1:9" ht="45">
+    <row r="290" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A290" s="25" t="s">
         <v>294</v>
       </c>
@@ -11165,11 +11138,11 @@
         <v>553</v>
       </c>
     </row>
-    <row r="291" spans="1:9">
+    <row r="291" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A291" s="3"/>
       <c r="B291" s="9"/>
     </row>
-    <row r="292" spans="1:9">
+    <row r="292" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A292" s="3"/>
       <c r="B292" s="9"/>
     </row>
@@ -11189,54 +11162,54 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A20:H52 A35:I290">
-    <cfRule type="expression" dxfId="13" priority="53">
+    <cfRule type="expression" dxfId="30" priority="53">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="54">
+    <cfRule type="expression" dxfId="29" priority="54">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="61">
+    <cfRule type="expression" dxfId="28" priority="61">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:H52 A35:I290">
-    <cfRule type="expression" dxfId="10" priority="7">
+    <cfRule type="expression" dxfId="27" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="8">
+    <cfRule type="expression" dxfId="26" priority="8">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="25" priority="9">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F290">
-    <cfRule type="expression" dxfId="7" priority="13">
+    <cfRule type="expression" dxfId="24" priority="13">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="14">
+    <cfRule type="expression" dxfId="23" priority="14">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:I52">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="22" priority="4">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="21" priority="5">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="20" priority="6">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:I52">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="19" priority="1">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="18" priority="2">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="17" priority="3">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update RS of MS-OXWSMTGS and MS-OXWSTASK according to the document of v20181001
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSTASK/MS-OXWSTASK_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSTASK/MS-OXWSTASK_RequirementSpecification.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Github\Interop-TestSuites\ExchangeWebServices\Docs\MS-OXWSTASK\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-xiahu\Desktop\test suite\Interop-TestSuites-1-master\ExchangeWebServices\Docs\MS-OXWSTASK\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D25184-9436-4AFB-9FAB-B6620E2794A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
+    <workbookView xWindow="21480" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$290</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$289</definedName>
     <definedName name="ExtensionList">Requirements!#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Requirements!$A:$A,Requirements!$19:$19</definedName>
     <definedName name="ScopeList">Requirements!#REF!</definedName>
@@ -25,15 +26,15 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="tmp2520" type="4" refreshedVersion="0" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="tmp2520" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\v-penj\AppData\Local\Temp\tmp2520.tmp" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1960" uniqueCount="646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1952" uniqueCount="643">
   <si>
     <t>Req ID</t>
   </si>
@@ -1650,9 +1651,6 @@
       &lt;soap:header message="tns:CopyItemSoapOut" part="ServerVersion" use="literal"/&gt;
    &lt;/wsdl:output&gt;
 &lt;/wsdl:operation&gt;</t>
-  </si>
-  <si>
-    <t>[In CopyItem Operation] tns:CopyItemSoapIn([MS-OXWSCORE] section 3.1.4.1.1.1): Specifies the SOAP message that defines the task item to be copied.</t>
   </si>
   <si>
     <t>[In CopyItem Operation] tns:CopyItemSoapOut ([MS-OXWSCORE] section 3.1.4.1.1.2): Specifies the SOAP message that is returned by the server in response.</t>
@@ -2477,19 +2475,10 @@
 &lt;/xs:complexType&gt;</t>
   </si>
   <si>
-    <t>[In t:TaskType Complex Type] The type of ActualWork is xs:int [XMLSCHEMA2] section 3.3.17.</t>
-  </si>
-  <si>
     <t>MS-OXWSTASK_R214001</t>
   </si>
   <si>
     <t>[In t:TaskType Complex Type] This element [AssignedTime] is read-only for the  client.</t>
-  </si>
-  <si>
-    <t>[In t:TaskType Complex Type] AssignedTime with xs:dateTime [XMLSCHEMA2] section 3.2.7 type specifies an instance of the DateTime structure that contains the time when a task is assigned to a contact.</t>
-  </si>
-  <si>
-    <t>[In t:TaskType Complex Type] The type of BillingInformation is xs:string [XMLSCHEMA2] section 3.2.1.</t>
   </si>
   <si>
     <t>[In t:TaskType Complex Type]The type of Companies is t:ArrayOfStringsType ([MS-OXWSCDATA] section 2.2.4.13).</t>
@@ -2588,9 +2577,6 @@
     <t>[In t:TaskDelegateStateType Simple Type] Accepted: Specifies that the task has been accepted. This value cannot be in the simple type.</t>
   </si>
   <si>
-    <t>[In t:TaskDelegateStateType Simple Type] Accepted: This value cannot be in the simple type.</t>
-  </si>
-  <si>
     <t>[In t:TaskDelegateStateType Simple Type] Declined: Specifies that the task has been declined.</t>
   </si>
   <si>
@@ -2603,9 +2589,6 @@
     <t>[In t:TaskDelegateStateType Simple Type] OwnNew: This value is also used for a task request message, whether it's in the owner's Sent Items folder or the delegate's Inbox folder.</t>
   </si>
   <si>
-    <t>MS-OXWSTASK_R91001</t>
-  </si>
-  <si>
     <t>[In t:TaskDelegateStateType Simple Type] OwnNew: Specifies that this is not a delegated task [or that the task request has been created but not sent].</t>
   </si>
   <si>
@@ -2669,15 +2652,6 @@
     <t>3.1.4.3.4.1</t>
   </si>
   <si>
-    <t>[In GetItem Operation] [tns:GetItemSoapOut ([MS-OXWSCORE] section 3.1.4.4.1.2)] The server returns a t:ItemResponseShapeType complex type element, as specified in [MS-OXWSCDATA] section 2.2.4.44, that contains properties associated with the task item.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[In CopyItem Operation] tns:CopyItemSoapIn ([MS-OXWSCORE] section 3.1.4.1.1.1): The CopyItem operation (as specified in [MS-OXWSCORE] section 3.1.4.1.1.1) that specifies the XML request MUST contain the t:TargetFolderIdType complex type (as specified in [MS-OXWSFOLD] section 2.2.4.16) and the t:ItemIdType complex type (as specified in [MS-OXWSCORE] section 2.2.4.25). </t>
-  </si>
-  <si>
-    <t>[In CopyItem Operation] tns:CopyItemSoapIn ([MS-OXWSCORE] section 3.1.4.1.1.1): All other type elements in t:NonEmptyArrayOfBaseItemIdsType element MUST NOT be included.</t>
-  </si>
-  <si>
     <t>[In MoveItem Operation] tns:MoveItemSoapIn  ([MS-OXWSCORE] section 3.1.4.7.1.1): All other type elements in t:NonEmptyArrayOfBaseItemIdsType element MUST be empty.</t>
   </si>
   <si>
@@ -2693,9 +2667,6 @@
     <t>[In t:TaskType Complex Type] ChangeCount: Specifies an integer value that specifies the number of times the task has changed since it was created.</t>
   </si>
   <si>
-    <t>6.0</t>
-  </si>
-  <si>
     <t>2.2.4.63</t>
   </si>
   <si>
@@ -2703,12 +2674,33 @@
   </si>
   <si>
     <t>[In t:RelativeYearlyRecurrencePatternType Complex Type] The element "DayOfWeekIndex" with type "t:DayOfWeekIndexType" specifies the week that is used in a relative yearly recurrence pattern.</t>
+  </si>
+  <si>
+    <t>[In t:TaskType Complex Type] The type of ActualWork is xs:int [XMLSCHEMA2/2] section 3.3.17.</t>
+  </si>
+  <si>
+    <t>[In t:TaskType Complex Type] AssignedTime with xs:dateTime [XMLSCHEMA2/2] section 3.2.7 type specifies an instance of the DateTime structure that contains the time when a task is assigned to a contact.</t>
+  </si>
+  <si>
+    <t>[In t:TaskType Complex Type] The type of BillingInformation is xs:string [XMLSCHEMA2/2] section 3.2.1.</t>
+  </si>
+  <si>
+    <t>[In CopyItem Operation] tns:CopyItemSoapIn([MS-OXWSCORE] section 3.1.4.1.1.1)%5BMS-OXWSCORE%5D.pdf: Specifies the SOAP message that defines the task item to be copied.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[In CopyItem Operation] tns:CopyItemSoapIn ([MS-OXWSCORE] section 3.1.4.1.1.1)%5BMS-OXWSCORE%5D.pdf: The CopyItem operation (as specified in [MS-OXWSCORE] section 3.1.4.1.1.1) that specifies the XML request MUST contain the t:TargetFolderIdType complex type (as specified in [MS-OXWSFOLD] section 2.2.4.16) and the t:ItemIdType complex type (as specified in [MS-OXWSCORE] section 2.2.4.25). </t>
+  </si>
+  <si>
+    <t>[In CopyItem Operation] tns:CopyItemSoapIn ([MS-OXWSCORE] section 3.1.4.1.1.1)%5BMS-OXWSCORE%5D.pdf: All other type elements in t:NonEmptyArrayOfBaseItemIdsType element MUST NOT be included.</t>
+  </si>
+  <si>
+    <t>[In GetItem Operation] [tns:GetItemSoapOut ([MS-OXWSCORE] section 3.1.4.4.1.2)] The server returns a  t:GetItemResponseType complex type element, which extends the BaseResponseMessageType complex type, as specified in [MS-OXWSCDATA] section 2.2.4.18, that contains properties associated with the task item.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.0.0"/>
@@ -3053,33 +3045,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3113,11 +3078,112 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="31">
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3437,80 +3503,6 @@
         <scheme val="none"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3640,34 +3632,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I290" tableType="xml" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" connectionId="1">
-  <autoFilter ref="A19:I290"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I289" tableType="xml" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29" connectionId="1">
+  <autoFilter ref="A19:I289" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="14">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="28">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="13">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="27">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="12">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="26">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="11">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="25">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="10">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="24">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="9">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="23">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="8">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="22">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="7">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="21">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="6">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="20">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -3676,12 +3668,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="A12:C15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+  <autoFilter ref="A12:C15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="2"/>
-    <tableColumn id="2" name="Test" dataDxfId="1"/>
-    <tableColumn id="3" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3763,6 +3755,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3798,6 +3807,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3973,11 +3999,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M292"/>
+  <dimension ref="A1:M291"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A220" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C224" sqref="C224"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -3996,7 +4024,7 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>27</v>
@@ -4008,7 +4036,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -4025,15 +4053,15 @@
       <c r="B3" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="44" t="s">
-        <v>642</v>
+      <c r="C3" s="63">
+        <v>8.1</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="34" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="35">
-        <v>42261</v>
+        <v>43445</v>
       </c>
       <c r="G3" s="36"/>
       <c r="H3" s="4"/>
@@ -4042,16 +4070,16 @@
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" ht="21">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
       <c r="I4" s="32"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -4063,13 +4091,13 @@
       <c r="B5" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="48"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="58"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
@@ -4077,16 +4105,16 @@
       <c r="A6" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="48"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="58"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
@@ -4094,16 +4122,16 @@
       <c r="A7" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="52"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="62"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
@@ -4111,16 +4139,16 @@
       <c r="A8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="51"/>
-      <c r="I8" s="52"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="62"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
@@ -4128,16 +4156,16 @@
       <c r="A9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="58"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="49"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
     </row>
@@ -4145,16 +4173,16 @@
       <c r="A10" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="58"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="49"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
     </row>
@@ -4162,16 +4190,16 @@
       <c r="A11" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="59" t="s">
-        <v>557</v>
-      </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="55"/>
+      <c r="B11" s="50" t="s">
+        <v>556</v>
+      </c>
+      <c r="C11" s="51"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="46"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
     </row>
@@ -4255,16 +4283,16 @@
       <c r="A16" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="61" t="s">
+      <c r="B16" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="62"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="54"/>
-      <c r="I16" s="55"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="46"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
     </row>
@@ -4272,16 +4300,16 @@
       <c r="A17" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="63" t="s">
-        <v>559</v>
-      </c>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="55"/>
+      <c r="B17" s="54" t="s">
+        <v>558</v>
+      </c>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="46"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
     </row>
@@ -4289,16 +4317,16 @@
       <c r="A18" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="53" t="s">
-        <v>558</v>
-      </c>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="54"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="55"/>
+      <c r="B18" s="44" t="s">
+        <v>557</v>
+      </c>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="46"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="M18" s="4"/>
@@ -4582,18 +4610,18 @@
         <v>17</v>
       </c>
       <c r="I29" s="20" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="30" spans="1:13" s="19" customFormat="1" ht="45">
       <c r="A30" s="18" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B30" s="20" t="s">
         <v>297</v>
       </c>
       <c r="C30" s="27" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D30" s="25"/>
       <c r="E30" s="25" t="s">
@@ -4609,7 +4637,7 @@
         <v>17</v>
       </c>
       <c r="I30" s="27" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="31" spans="1:13" s="19" customFormat="1" ht="30">
@@ -4795,7 +4823,7 @@
         <v>299</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D38" s="25"/>
       <c r="E38" s="25" t="s">
@@ -5020,7 +5048,7 @@
         <v>302</v>
       </c>
       <c r="C47" s="27" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D47" s="25"/>
       <c r="E47" s="25" t="s">
@@ -5195,7 +5223,7 @@
         <v>32</v>
       </c>
       <c r="C54" s="27" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D54" s="25"/>
       <c r="E54" s="25" t="s">
@@ -5245,7 +5273,7 @@
         <v>303</v>
       </c>
       <c r="C56" s="27" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D56" s="25"/>
       <c r="E56" s="25" t="s">
@@ -5295,7 +5323,7 @@
         <v>304</v>
       </c>
       <c r="C58" s="27" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D58" s="25"/>
       <c r="E58" s="25" t="s">
@@ -5445,7 +5473,7 @@
         <v>306</v>
       </c>
       <c r="C64" s="27" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D64" s="25"/>
       <c r="E64" s="25" t="s">
@@ -5470,7 +5498,7 @@
         <v>307</v>
       </c>
       <c r="C65" s="27" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D65" s="25"/>
       <c r="E65" s="25" t="s">
@@ -5495,7 +5523,7 @@
         <v>307</v>
       </c>
       <c r="C66" s="27" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D66" s="25"/>
       <c r="E66" s="25" t="s">
@@ -5537,15 +5565,15 @@
       </c>
       <c r="I67" s="27"/>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" ht="30">
       <c r="A68" s="25" t="s">
         <v>82</v>
       </c>
       <c r="B68" s="26" t="s">
         <v>307</v>
       </c>
-      <c r="C68" s="27" t="s">
-        <v>574</v>
+      <c r="C68" s="16" t="s">
+        <v>636</v>
       </c>
       <c r="D68" s="25"/>
       <c r="E68" s="25" t="s">
@@ -5594,8 +5622,8 @@
       <c r="B70" s="26" t="s">
         <v>307</v>
       </c>
-      <c r="C70" s="27" t="s">
-        <v>577</v>
+      <c r="C70" s="16" t="s">
+        <v>637</v>
       </c>
       <c r="D70" s="25"/>
       <c r="E70" s="25" t="s">
@@ -5614,13 +5642,13 @@
     </row>
     <row r="71" spans="1:9">
       <c r="A71" s="25" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B71" s="26" t="s">
         <v>307</v>
       </c>
       <c r="C71" s="27" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="D71" s="25"/>
       <c r="E71" s="25" t="s">
@@ -5644,8 +5672,8 @@
       <c r="B72" s="26" t="s">
         <v>307</v>
       </c>
-      <c r="C72" s="27" t="s">
-        <v>578</v>
+      <c r="C72" s="16" t="s">
+        <v>638</v>
       </c>
       <c r="D72" s="25"/>
       <c r="E72" s="25" t="s">
@@ -5720,7 +5748,7 @@
         <v>307</v>
       </c>
       <c r="C75" s="27" t="s">
-        <v>641</v>
+        <v>632</v>
       </c>
       <c r="D75" s="25"/>
       <c r="E75" s="25" t="s">
@@ -5739,13 +5767,13 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" s="25" t="s">
-        <v>639</v>
+        <v>630</v>
       </c>
       <c r="B76" s="26" t="s">
         <v>307</v>
       </c>
       <c r="C76" s="27" t="s">
-        <v>640</v>
+        <v>631</v>
       </c>
       <c r="D76" s="25"/>
       <c r="E76" s="25" t="s">
@@ -5770,7 +5798,7 @@
         <v>307</v>
       </c>
       <c r="C77" s="27" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="D77" s="25"/>
       <c r="E77" s="25" t="s">
@@ -5964,13 +5992,13 @@
     </row>
     <row r="85" spans="1:9">
       <c r="A85" s="25" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="B85" s="26" t="s">
         <v>307</v>
       </c>
       <c r="C85" s="27" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="D85" s="25"/>
       <c r="E85" s="25" t="s">
@@ -6045,7 +6073,7 @@
         <v>307</v>
       </c>
       <c r="C88" s="27" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="D88" s="25"/>
       <c r="E88" s="25" t="s">
@@ -6064,13 +6092,13 @@
     </row>
     <row r="89" spans="1:9" ht="30">
       <c r="A89" s="25" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="B89" s="26" t="s">
         <v>307</v>
       </c>
       <c r="C89" s="27" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="D89" s="25"/>
       <c r="E89" s="25" t="s">
@@ -6095,7 +6123,7 @@
         <v>307</v>
       </c>
       <c r="C90" s="27" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="D90" s="25"/>
       <c r="E90" s="25" t="s">
@@ -6148,7 +6176,7 @@
         <v>390</v>
       </c>
       <c r="D92" s="25" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E92" s="25" t="s">
         <v>19</v>
@@ -6175,7 +6203,7 @@
         <v>391</v>
       </c>
       <c r="D93" s="25" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E93" s="25" t="s">
         <v>19</v>
@@ -6193,13 +6221,13 @@
     </row>
     <row r="94" spans="1:9">
       <c r="A94" s="25" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="B94" s="26" t="s">
         <v>307</v>
       </c>
       <c r="C94" s="27" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="D94" s="25"/>
       <c r="E94" s="25" t="s">
@@ -6277,7 +6305,7 @@
         <v>394</v>
       </c>
       <c r="D97" s="25" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="E97" s="25" t="s">
         <v>19</v>
@@ -6304,7 +6332,7 @@
         <v>395</v>
       </c>
       <c r="D98" s="25" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="E98" s="25" t="s">
         <v>19</v>
@@ -6322,13 +6350,13 @@
     </row>
     <row r="99" spans="1:9">
       <c r="A99" s="25" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="B99" s="26" t="s">
         <v>307</v>
       </c>
       <c r="C99" s="27" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="D99" s="25"/>
       <c r="E99" s="25" t="s">
@@ -6372,13 +6400,13 @@
     </row>
     <row r="101" spans="1:9">
       <c r="A101" s="25" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="B101" s="26" t="s">
         <v>307</v>
       </c>
       <c r="C101" s="27" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="D101" s="25"/>
       <c r="E101" s="25" t="s">
@@ -6472,13 +6500,13 @@
     </row>
     <row r="105" spans="1:9" ht="30">
       <c r="A105" s="25" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="B105" s="26" t="s">
         <v>307</v>
       </c>
       <c r="C105" s="27" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="D105" s="25"/>
       <c r="E105" s="25" t="s">
@@ -6503,7 +6531,7 @@
         <v>307</v>
       </c>
       <c r="C106" s="27" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="D106" s="25"/>
       <c r="E106" s="25" t="s">
@@ -6553,7 +6581,7 @@
         <v>307</v>
       </c>
       <c r="C108" s="27" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="D108" s="25"/>
       <c r="E108" s="25" t="s">
@@ -6747,13 +6775,13 @@
     </row>
     <row r="116" spans="1:9">
       <c r="A116" s="25" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="B116" s="26" t="s">
         <v>307</v>
       </c>
       <c r="C116" s="27" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="D116" s="25"/>
       <c r="E116" s="25" t="s">
@@ -6822,13 +6850,13 @@
     </row>
     <row r="119" spans="1:9" ht="30">
       <c r="A119" s="25" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="B119" s="26" t="s">
         <v>307</v>
       </c>
       <c r="C119" s="27" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="D119" s="25"/>
       <c r="E119" s="25" t="s">
@@ -6847,13 +6875,13 @@
     </row>
     <row r="120" spans="1:9" ht="30">
       <c r="A120" s="25" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="B120" s="26" t="s">
         <v>307</v>
       </c>
       <c r="C120" s="27" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="D120" s="25"/>
       <c r="E120" s="25" t="s">
@@ -6872,13 +6900,13 @@
     </row>
     <row r="121" spans="1:9" ht="60">
       <c r="A121" s="25" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="B121" s="26" t="s">
         <v>307</v>
       </c>
       <c r="C121" s="27" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="D121" s="25"/>
       <c r="E121" s="25" t="s">
@@ -6928,7 +6956,7 @@
         <v>308</v>
       </c>
       <c r="C123" s="27" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="D123" s="25"/>
       <c r="E123" s="25" t="s">
@@ -6978,7 +7006,7 @@
         <v>309</v>
       </c>
       <c r="C125" s="27" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="D125" s="25"/>
       <c r="E125" s="25" t="s">
@@ -7228,7 +7256,7 @@
         <v>311</v>
       </c>
       <c r="C135" s="27" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="D135" s="25"/>
       <c r="E135" s="25" t="s">
@@ -7247,13 +7275,13 @@
     </row>
     <row r="136" spans="1:9" ht="30">
       <c r="A136" s="25" t="s">
-        <v>612</v>
+        <v>144</v>
       </c>
       <c r="B136" s="26" t="s">
         <v>311</v>
       </c>
       <c r="C136" s="27" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="D136" s="25"/>
       <c r="E136" s="25" t="s">
@@ -7270,15 +7298,15 @@
       </c>
       <c r="I136" s="27"/>
     </row>
-    <row r="137" spans="1:9" ht="30">
+    <row r="137" spans="1:9">
       <c r="A137" s="25" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B137" s="26" t="s">
         <v>311</v>
       </c>
       <c r="C137" s="27" t="s">
-        <v>608</v>
+        <v>424</v>
       </c>
       <c r="D137" s="25"/>
       <c r="E137" s="25" t="s">
@@ -7297,13 +7325,13 @@
     </row>
     <row r="138" spans="1:9">
       <c r="A138" s="25" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B138" s="26" t="s">
         <v>311</v>
       </c>
       <c r="C138" s="27" t="s">
-        <v>424</v>
+        <v>604</v>
       </c>
       <c r="D138" s="25"/>
       <c r="E138" s="25" t="s">
@@ -7320,15 +7348,15 @@
       </c>
       <c r="I138" s="27"/>
     </row>
-    <row r="139" spans="1:9">
+    <row r="139" spans="1:9" ht="30">
       <c r="A139" s="25" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B139" s="26" t="s">
         <v>311</v>
       </c>
       <c r="C139" s="27" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="D139" s="25"/>
       <c r="E139" s="25" t="s">
@@ -7347,13 +7375,13 @@
     </row>
     <row r="140" spans="1:9" ht="30">
       <c r="A140" s="25" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B140" s="26" t="s">
         <v>311</v>
       </c>
       <c r="C140" s="27" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="D140" s="25"/>
       <c r="E140" s="25" t="s">
@@ -7372,13 +7400,13 @@
     </row>
     <row r="141" spans="1:9" ht="30">
       <c r="A141" s="25" t="s">
-        <v>148</v>
+        <v>609</v>
       </c>
       <c r="B141" s="26" t="s">
         <v>311</v>
       </c>
       <c r="C141" s="27" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="D141" s="25"/>
       <c r="E141" s="25" t="s">
@@ -7395,22 +7423,22 @@
       </c>
       <c r="I141" s="27"/>
     </row>
-    <row r="142" spans="1:9" ht="30">
+    <row r="142" spans="1:9" ht="45">
       <c r="A142" s="25" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="B142" s="26" t="s">
         <v>311</v>
       </c>
       <c r="C142" s="27" t="s">
-        <v>614</v>
+        <v>606</v>
       </c>
       <c r="D142" s="25"/>
       <c r="E142" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F142" s="25" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G142" s="25" t="s">
         <v>15</v>
@@ -7420,40 +7448,40 @@
       </c>
       <c r="I142" s="27"/>
     </row>
-    <row r="143" spans="1:9" ht="45">
+    <row r="143" spans="1:9" ht="255">
       <c r="A143" s="25" t="s">
-        <v>616</v>
+        <v>149</v>
       </c>
       <c r="B143" s="26" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C143" s="27" t="s">
-        <v>611</v>
+        <v>425</v>
       </c>
       <c r="D143" s="25"/>
       <c r="E143" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F143" s="25" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G143" s="25" t="s">
         <v>15</v>
       </c>
       <c r="H143" s="25" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I143" s="27"/>
     </row>
-    <row r="144" spans="1:9" ht="255">
+    <row r="144" spans="1:9" ht="45">
       <c r="A144" s="25" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B144" s="26" t="s">
         <v>312</v>
       </c>
       <c r="C144" s="27" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D144" s="25"/>
       <c r="E144" s="25" t="s">
@@ -7463,22 +7491,22 @@
         <v>3</v>
       </c>
       <c r="G144" s="25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H144" s="25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I144" s="27"/>
     </row>
-    <row r="145" spans="1:9" ht="45">
+    <row r="145" spans="1:9">
       <c r="A145" s="25" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B145" s="26" t="s">
         <v>312</v>
       </c>
       <c r="C145" s="27" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="D145" s="25"/>
       <c r="E145" s="25" t="s">
@@ -7488,22 +7516,22 @@
         <v>3</v>
       </c>
       <c r="G145" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H145" s="25" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I145" s="27"/>
     </row>
     <row r="146" spans="1:9">
       <c r="A146" s="25" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B146" s="26" t="s">
         <v>312</v>
       </c>
       <c r="C146" s="27" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="D146" s="25"/>
       <c r="E146" s="25" t="s">
@@ -7522,13 +7550,13 @@
     </row>
     <row r="147" spans="1:9">
       <c r="A147" s="25" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B147" s="26" t="s">
         <v>312</v>
       </c>
       <c r="C147" s="27" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="D147" s="25"/>
       <c r="E147" s="25" t="s">
@@ -7547,13 +7575,13 @@
     </row>
     <row r="148" spans="1:9">
       <c r="A148" s="25" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B148" s="26" t="s">
         <v>312</v>
       </c>
       <c r="C148" s="27" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="D148" s="25"/>
       <c r="E148" s="25" t="s">
@@ -7570,15 +7598,15 @@
       </c>
       <c r="I148" s="27"/>
     </row>
-    <row r="149" spans="1:9">
+    <row r="149" spans="1:9" ht="30">
       <c r="A149" s="25" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B149" s="26" t="s">
         <v>312</v>
       </c>
       <c r="C149" s="27" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D149" s="25"/>
       <c r="E149" s="25" t="s">
@@ -7597,13 +7625,13 @@
     </row>
     <row r="150" spans="1:9" ht="30">
       <c r="A150" s="25" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B150" s="26" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C150" s="27" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="D150" s="25"/>
       <c r="E150" s="25" t="s">
@@ -7613,22 +7641,22 @@
         <v>3</v>
       </c>
       <c r="G150" s="25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H150" s="25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I150" s="27"/>
     </row>
-    <row r="151" spans="1:9" ht="30">
+    <row r="151" spans="1:9" ht="45">
       <c r="A151" s="25" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B151" s="26" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C151" s="27" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="D151" s="25"/>
       <c r="E151" s="25" t="s">
@@ -7645,15 +7673,15 @@
       </c>
       <c r="I151" s="27"/>
     </row>
-    <row r="152" spans="1:9" ht="45">
+    <row r="152" spans="1:9" ht="30">
       <c r="A152" s="25" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B152" s="26" t="s">
         <v>314</v>
       </c>
       <c r="C152" s="27" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D152" s="25"/>
       <c r="E152" s="25" t="s">
@@ -7672,13 +7700,13 @@
     </row>
     <row r="153" spans="1:9" ht="30">
       <c r="A153" s="25" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B153" s="26" t="s">
         <v>314</v>
       </c>
       <c r="C153" s="27" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="D153" s="25"/>
       <c r="E153" s="25" t="s">
@@ -7695,15 +7723,15 @@
       </c>
       <c r="I153" s="27"/>
     </row>
-    <row r="154" spans="1:9" ht="30">
+    <row r="154" spans="1:9" ht="409.5">
       <c r="A154" s="25" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B154" s="26" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C154" s="27" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="D154" s="25"/>
       <c r="E154" s="25" t="s">
@@ -7713,22 +7741,22 @@
         <v>3</v>
       </c>
       <c r="G154" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H154" s="25" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I154" s="27"/>
     </row>
-    <row r="155" spans="1:9" ht="409.5">
+    <row r="155" spans="1:9" ht="75">
       <c r="A155" s="25" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B155" s="26" t="s">
         <v>315</v>
       </c>
       <c r="C155" s="27" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="D155" s="25"/>
       <c r="E155" s="25" t="s">
@@ -7738,22 +7766,22 @@
         <v>3</v>
       </c>
       <c r="G155" s="25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H155" s="25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I155" s="27"/>
     </row>
-    <row r="156" spans="1:9" ht="75">
+    <row r="156" spans="1:9" ht="30">
       <c r="A156" s="25" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B156" s="26" t="s">
         <v>315</v>
       </c>
       <c r="C156" s="27" t="s">
-        <v>437</v>
+        <v>611</v>
       </c>
       <c r="D156" s="25"/>
       <c r="E156" s="25" t="s">
@@ -7763,22 +7791,22 @@
         <v>3</v>
       </c>
       <c r="G156" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H156" s="25" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I156" s="27"/>
     </row>
     <row r="157" spans="1:9" ht="30">
       <c r="A157" s="25" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B157" s="26" t="s">
         <v>315</v>
       </c>
       <c r="C157" s="27" t="s">
-        <v>617</v>
+        <v>438</v>
       </c>
       <c r="D157" s="25"/>
       <c r="E157" s="25" t="s">
@@ -7797,13 +7825,13 @@
     </row>
     <row r="158" spans="1:9" ht="30">
       <c r="A158" s="25" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B158" s="26" t="s">
         <v>315</v>
       </c>
       <c r="C158" s="27" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="D158" s="25"/>
       <c r="E158" s="25" t="s">
@@ -7822,13 +7850,13 @@
     </row>
     <row r="159" spans="1:9" ht="30">
       <c r="A159" s="25" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B159" s="26" t="s">
         <v>315</v>
       </c>
       <c r="C159" s="27" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="D159" s="25"/>
       <c r="E159" s="25" t="s">
@@ -7847,13 +7875,13 @@
     </row>
     <row r="160" spans="1:9" ht="30">
       <c r="A160" s="25" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B160" s="26" t="s">
         <v>315</v>
       </c>
       <c r="C160" s="27" t="s">
-        <v>440</v>
+        <v>612</v>
       </c>
       <c r="D160" s="25"/>
       <c r="E160" s="25" t="s">
@@ -7872,13 +7900,13 @@
     </row>
     <row r="161" spans="1:9" ht="30">
       <c r="A161" s="25" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B161" s="26" t="s">
         <v>315</v>
       </c>
       <c r="C161" s="27" t="s">
-        <v>618</v>
+        <v>441</v>
       </c>
       <c r="D161" s="25"/>
       <c r="E161" s="25" t="s">
@@ -7897,13 +7925,13 @@
     </row>
     <row r="162" spans="1:9" ht="30">
       <c r="A162" s="25" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B162" s="26" t="s">
         <v>315</v>
       </c>
       <c r="C162" s="27" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="D162" s="25"/>
       <c r="E162" s="25" t="s">
@@ -7922,13 +7950,13 @@
     </row>
     <row r="163" spans="1:9" ht="30">
       <c r="A163" s="25" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B163" s="26" t="s">
         <v>315</v>
       </c>
       <c r="C163" s="27" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="D163" s="25"/>
       <c r="E163" s="25" t="s">
@@ -7947,13 +7975,13 @@
     </row>
     <row r="164" spans="1:9" ht="30">
       <c r="A164" s="25" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B164" s="26" t="s">
         <v>315</v>
       </c>
       <c r="C164" s="27" t="s">
-        <v>443</v>
+        <v>613</v>
       </c>
       <c r="D164" s="25"/>
       <c r="E164" s="25" t="s">
@@ -7972,13 +8000,13 @@
     </row>
     <row r="165" spans="1:9" ht="30">
       <c r="A165" s="25" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B165" s="26" t="s">
         <v>315</v>
       </c>
       <c r="C165" s="27" t="s">
-        <v>619</v>
+        <v>444</v>
       </c>
       <c r="D165" s="25"/>
       <c r="E165" s="25" t="s">
@@ -7997,13 +8025,13 @@
     </row>
     <row r="166" spans="1:9" ht="30">
       <c r="A166" s="25" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B166" s="26" t="s">
         <v>315</v>
       </c>
       <c r="C166" s="27" t="s">
-        <v>444</v>
+        <v>614</v>
       </c>
       <c r="D166" s="25"/>
       <c r="E166" s="25" t="s">
@@ -8022,13 +8050,13 @@
     </row>
     <row r="167" spans="1:9" ht="30">
       <c r="A167" s="25" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B167" s="26" t="s">
         <v>315</v>
       </c>
       <c r="C167" s="27" t="s">
-        <v>620</v>
+        <v>445</v>
       </c>
       <c r="D167" s="25"/>
       <c r="E167" s="25" t="s">
@@ -8047,13 +8075,13 @@
     </row>
     <row r="168" spans="1:9" ht="30">
       <c r="A168" s="25" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B168" s="26" t="s">
         <v>315</v>
       </c>
       <c r="C168" s="27" t="s">
-        <v>445</v>
+        <v>615</v>
       </c>
       <c r="D168" s="25"/>
       <c r="E168" s="25" t="s">
@@ -8072,13 +8100,13 @@
     </row>
     <row r="169" spans="1:9" ht="30">
       <c r="A169" s="25" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B169" s="26" t="s">
         <v>315</v>
       </c>
       <c r="C169" s="27" t="s">
-        <v>621</v>
+        <v>446</v>
       </c>
       <c r="D169" s="25"/>
       <c r="E169" s="25" t="s">
@@ -8097,13 +8125,13 @@
     </row>
     <row r="170" spans="1:9" ht="30">
       <c r="A170" s="25" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B170" s="26" t="s">
         <v>315</v>
       </c>
       <c r="C170" s="27" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="D170" s="25"/>
       <c r="E170" s="25" t="s">
@@ -8122,13 +8150,13 @@
     </row>
     <row r="171" spans="1:9" ht="30">
       <c r="A171" s="25" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B171" s="26" t="s">
         <v>315</v>
       </c>
       <c r="C171" s="27" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D171" s="25"/>
       <c r="E171" s="25" t="s">
@@ -8147,13 +8175,13 @@
     </row>
     <row r="172" spans="1:9" ht="30">
       <c r="A172" s="25" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B172" s="26" t="s">
         <v>315</v>
       </c>
       <c r="C172" s="27" t="s">
-        <v>448</v>
+        <v>616</v>
       </c>
       <c r="D172" s="25"/>
       <c r="E172" s="25" t="s">
@@ -8172,13 +8200,13 @@
     </row>
     <row r="173" spans="1:9" ht="30">
       <c r="A173" s="25" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B173" s="26" t="s">
         <v>315</v>
       </c>
       <c r="C173" s="27" t="s">
-        <v>622</v>
+        <v>449</v>
       </c>
       <c r="D173" s="25"/>
       <c r="E173" s="25" t="s">
@@ -8197,13 +8225,13 @@
     </row>
     <row r="174" spans="1:9" ht="30">
       <c r="A174" s="25" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B174" s="26" t="s">
         <v>315</v>
       </c>
       <c r="C174" s="27" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="D174" s="25"/>
       <c r="E174" s="25" t="s">
@@ -8222,13 +8250,13 @@
     </row>
     <row r="175" spans="1:9" ht="30">
       <c r="A175" s="25" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B175" s="26" t="s">
         <v>315</v>
       </c>
       <c r="C175" s="27" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="D175" s="25"/>
       <c r="E175" s="25" t="s">
@@ -8247,13 +8275,13 @@
     </row>
     <row r="176" spans="1:9" ht="30">
       <c r="A176" s="25" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B176" s="26" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C176" s="27" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="D176" s="25"/>
       <c r="E176" s="25" t="s">
@@ -8263,22 +8291,22 @@
         <v>3</v>
       </c>
       <c r="G176" s="25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H176" s="25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I176" s="27"/>
     </row>
     <row r="177" spans="1:9" ht="30">
       <c r="A177" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B177" s="26" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C177" s="27" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="D177" s="25"/>
       <c r="E177" s="25" t="s">
@@ -8297,20 +8325,20 @@
     </row>
     <row r="178" spans="1:9" ht="30">
       <c r="A178" s="25" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B178" s="26" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C178" s="27" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="D178" s="25"/>
       <c r="E178" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F178" s="25" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G178" s="25" t="s">
         <v>16</v>
@@ -8322,13 +8350,13 @@
     </row>
     <row r="179" spans="1:9" ht="30">
       <c r="A179" s="25" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B179" s="26" t="s">
         <v>318</v>
       </c>
       <c r="C179" s="27" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="D179" s="25"/>
       <c r="E179" s="25" t="s">
@@ -8345,22 +8373,22 @@
       </c>
       <c r="I179" s="27"/>
     </row>
-    <row r="180" spans="1:9" ht="30">
+    <row r="180" spans="1:9" ht="45">
       <c r="A180" s="25" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B180" s="26" t="s">
         <v>318</v>
       </c>
       <c r="C180" s="27" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="D180" s="25"/>
       <c r="E180" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F180" s="25" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G180" s="25" t="s">
         <v>16</v>
@@ -8370,22 +8398,22 @@
       </c>
       <c r="I180" s="27"/>
     </row>
-    <row r="181" spans="1:9" ht="45">
+    <row r="181" spans="1:9" ht="30">
       <c r="A181" s="25" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B181" s="26" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C181" s="27" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="D181" s="25"/>
       <c r="E181" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F181" s="25" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G181" s="25" t="s">
         <v>16</v>
@@ -8397,20 +8425,20 @@
     </row>
     <row r="182" spans="1:9" ht="30">
       <c r="A182" s="25" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B182" s="26" t="s">
         <v>319</v>
       </c>
       <c r="C182" s="27" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="D182" s="25"/>
       <c r="E182" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F182" s="25" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G182" s="25" t="s">
         <v>16</v>
@@ -8420,15 +8448,15 @@
       </c>
       <c r="I182" s="27"/>
     </row>
-    <row r="183" spans="1:9" ht="30">
+    <row r="183" spans="1:9" ht="45">
       <c r="A183" s="25" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B183" s="26" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C183" s="27" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="D183" s="25"/>
       <c r="E183" s="25" t="s">
@@ -8445,15 +8473,15 @@
       </c>
       <c r="I183" s="27"/>
     </row>
-    <row r="184" spans="1:9" ht="45">
+    <row r="184" spans="1:9" ht="30">
       <c r="A184" s="25" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B184" s="26" t="s">
         <v>320</v>
       </c>
       <c r="C184" s="27" t="s">
-        <v>459</v>
+        <v>617</v>
       </c>
       <c r="D184" s="25"/>
       <c r="E184" s="25" t="s">
@@ -8472,13 +8500,13 @@
     </row>
     <row r="185" spans="1:9" ht="30">
       <c r="A185" s="25" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B185" s="26" t="s">
         <v>320</v>
       </c>
       <c r="C185" s="27" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="D185" s="25"/>
       <c r="E185" s="25" t="s">
@@ -8497,13 +8525,13 @@
     </row>
     <row r="186" spans="1:9" ht="30">
       <c r="A186" s="25" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B186" s="26" t="s">
         <v>320</v>
       </c>
       <c r="C186" s="27" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="D186" s="25"/>
       <c r="E186" s="25" t="s">
@@ -8522,13 +8550,13 @@
     </row>
     <row r="187" spans="1:9" ht="30">
       <c r="A187" s="25" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B187" s="26" t="s">
         <v>320</v>
       </c>
       <c r="C187" s="27" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="D187" s="25"/>
       <c r="E187" s="25" t="s">
@@ -8547,13 +8575,13 @@
     </row>
     <row r="188" spans="1:9" ht="30">
       <c r="A188" s="25" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B188" s="26" t="s">
         <v>320</v>
       </c>
       <c r="C188" s="27" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="D188" s="25"/>
       <c r="E188" s="25" t="s">
@@ -8572,13 +8600,13 @@
     </row>
     <row r="189" spans="1:9" ht="30">
       <c r="A189" s="25" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B189" s="26" t="s">
         <v>320</v>
       </c>
       <c r="C189" s="27" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="D189" s="25"/>
       <c r="E189" s="25" t="s">
@@ -8597,13 +8625,13 @@
     </row>
     <row r="190" spans="1:9" ht="30">
       <c r="A190" s="25" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B190" s="26" t="s">
-        <v>320</v>
+        <v>33</v>
       </c>
       <c r="C190" s="27" t="s">
-        <v>628</v>
+        <v>460</v>
       </c>
       <c r="D190" s="25"/>
       <c r="E190" s="25" t="s">
@@ -8620,15 +8648,15 @@
       </c>
       <c r="I190" s="27"/>
     </row>
-    <row r="191" spans="1:9" ht="30">
+    <row r="191" spans="1:9" ht="75">
       <c r="A191" s="25" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B191" s="26" t="s">
         <v>33</v>
       </c>
       <c r="C191" s="27" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="D191" s="25"/>
       <c r="E191" s="25" t="s">
@@ -8638,22 +8666,22 @@
         <v>3</v>
       </c>
       <c r="G191" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H191" s="25" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I191" s="27"/>
     </row>
-    <row r="192" spans="1:9" ht="75">
+    <row r="192" spans="1:9" ht="240">
       <c r="A192" s="25" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B192" s="26" t="s">
         <v>33</v>
       </c>
       <c r="C192" s="27" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="D192" s="25"/>
       <c r="E192" s="25" t="s">
@@ -8670,40 +8698,40 @@
       </c>
       <c r="I192" s="27"/>
     </row>
-    <row r="193" spans="1:9" ht="240">
+    <row r="193" spans="1:9" ht="30">
       <c r="A193" s="25" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B193" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="C193" s="27" t="s">
-        <v>462</v>
+      <c r="C193" s="16" t="s">
+        <v>639</v>
       </c>
       <c r="D193" s="25"/>
       <c r="E193" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F193" s="25" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G193" s="25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H193" s="25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I193" s="27"/>
     </row>
-    <row r="194" spans="1:9" ht="30">
+    <row r="194" spans="1:9" ht="75">
       <c r="A194" s="25" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B194" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="C194" s="27" t="s">
-        <v>463</v>
+      <c r="C194" s="16" t="s">
+        <v>640</v>
       </c>
       <c r="D194" s="25"/>
       <c r="E194" s="25" t="s">
@@ -8713,22 +8741,22 @@
         <v>7</v>
       </c>
       <c r="G194" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H194" s="25" t="s">
         <v>18</v>
       </c>
       <c r="I194" s="27"/>
     </row>
-    <row r="195" spans="1:9" ht="75">
+    <row r="195" spans="1:9" ht="45">
       <c r="A195" s="25" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B195" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="C195" s="27" t="s">
-        <v>635</v>
+      <c r="C195" s="16" t="s">
+        <v>641</v>
       </c>
       <c r="D195" s="25"/>
       <c r="E195" s="25" t="s">
@@ -8745,25 +8773,25 @@
       </c>
       <c r="I195" s="27"/>
     </row>
-    <row r="196" spans="1:9" ht="45">
+    <row r="196" spans="1:9" ht="30">
       <c r="A196" s="25" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B196" s="26" t="s">
         <v>33</v>
       </c>
       <c r="C196" s="27" t="s">
-        <v>636</v>
+        <v>463</v>
       </c>
       <c r="D196" s="25"/>
       <c r="E196" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F196" s="25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G196" s="25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H196" s="25" t="s">
         <v>18</v>
@@ -8772,10 +8800,10 @@
     </row>
     <row r="197" spans="1:9" ht="30">
       <c r="A197" s="25" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B197" s="26" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C197" s="27" t="s">
         <v>464</v>
@@ -8785,7 +8813,7 @@
         <v>19</v>
       </c>
       <c r="F197" s="25" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G197" s="25" t="s">
         <v>16</v>
@@ -8795,9 +8823,9 @@
       </c>
       <c r="I197" s="27"/>
     </row>
-    <row r="198" spans="1:9" ht="30">
+    <row r="198" spans="1:9" ht="75">
       <c r="A198" s="25" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B198" s="26" t="s">
         <v>34</v>
@@ -8813,16 +8841,16 @@
         <v>3</v>
       </c>
       <c r="G198" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H198" s="25" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I198" s="27"/>
     </row>
-    <row r="199" spans="1:9" ht="75">
+    <row r="199" spans="1:9" ht="255">
       <c r="A199" s="25" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B199" s="26" t="s">
         <v>34</v>
@@ -8845,9 +8873,9 @@
       </c>
       <c r="I199" s="27"/>
     </row>
-    <row r="200" spans="1:9" ht="255">
+    <row r="200" spans="1:9" ht="30">
       <c r="A200" s="25" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B200" s="26" t="s">
         <v>34</v>
@@ -8860,25 +8888,25 @@
         <v>19</v>
       </c>
       <c r="F200" s="25" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G200" s="25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H200" s="25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I200" s="27"/>
     </row>
-    <row r="201" spans="1:9" ht="30">
+    <row r="201" spans="1:9" ht="75">
       <c r="A201" s="25" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B201" s="26" t="s">
         <v>34</v>
       </c>
       <c r="C201" s="27" t="s">
-        <v>468</v>
+        <v>623</v>
       </c>
       <c r="D201" s="25"/>
       <c r="E201" s="25" t="s">
@@ -8888,22 +8916,22 @@
         <v>7</v>
       </c>
       <c r="G201" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H201" s="25" t="s">
         <v>18</v>
       </c>
       <c r="I201" s="27"/>
     </row>
-    <row r="202" spans="1:9" ht="75">
+    <row r="202" spans="1:9" ht="30">
       <c r="A202" s="25" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B202" s="26" t="s">
         <v>34</v>
       </c>
       <c r="C202" s="27" t="s">
-        <v>629</v>
+        <v>468</v>
       </c>
       <c r="D202" s="25"/>
       <c r="E202" s="25" t="s">
@@ -8922,7 +8950,7 @@
     </row>
     <row r="203" spans="1:9" ht="30">
       <c r="A203" s="25" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B203" s="26" t="s">
         <v>34</v>
@@ -8935,10 +8963,10 @@
         <v>19</v>
       </c>
       <c r="F203" s="25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G203" s="25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H203" s="25" t="s">
         <v>18</v>
@@ -8947,10 +8975,10 @@
     </row>
     <row r="204" spans="1:9" ht="30">
       <c r="A204" s="25" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B204" s="26" t="s">
-        <v>34</v>
+        <v>321</v>
       </c>
       <c r="C204" s="27" t="s">
         <v>470</v>
@@ -8960,7 +8988,7 @@
         <v>19</v>
       </c>
       <c r="F204" s="25" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G204" s="25" t="s">
         <v>16</v>
@@ -8970,9 +8998,9 @@
       </c>
       <c r="I204" s="27"/>
     </row>
-    <row r="205" spans="1:9" ht="30">
+    <row r="205" spans="1:9" ht="75">
       <c r="A205" s="25" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B205" s="26" t="s">
         <v>321</v>
@@ -8988,16 +9016,16 @@
         <v>3</v>
       </c>
       <c r="G205" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H205" s="25" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I205" s="27"/>
     </row>
-    <row r="206" spans="1:9" ht="75">
+    <row r="206" spans="1:9" ht="240">
       <c r="A206" s="25" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B206" s="26" t="s">
         <v>321</v>
@@ -9020,9 +9048,9 @@
       </c>
       <c r="I206" s="27"/>
     </row>
-    <row r="207" spans="1:9" ht="240">
+    <row r="207" spans="1:9" ht="30">
       <c r="A207" s="25" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B207" s="26" t="s">
         <v>321</v>
@@ -9035,25 +9063,25 @@
         <v>19</v>
       </c>
       <c r="F207" s="25" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G207" s="25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H207" s="25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I207" s="27"/>
     </row>
-    <row r="208" spans="1:9" ht="30">
+    <row r="208" spans="1:9" ht="75">
       <c r="A208" s="25" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B208" s="26" t="s">
         <v>321</v>
       </c>
       <c r="C208" s="27" t="s">
-        <v>474</v>
+        <v>624</v>
       </c>
       <c r="D208" s="25"/>
       <c r="E208" s="25" t="s">
@@ -9063,22 +9091,22 @@
         <v>7</v>
       </c>
       <c r="G208" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H208" s="25" t="s">
         <v>18</v>
       </c>
       <c r="I208" s="27"/>
     </row>
-    <row r="209" spans="1:9" ht="75">
+    <row r="209" spans="1:9" ht="30">
       <c r="A209" s="25" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B209" s="26" t="s">
         <v>321</v>
       </c>
       <c r="C209" s="27" t="s">
-        <v>630</v>
+        <v>474</v>
       </c>
       <c r="D209" s="25"/>
       <c r="E209" s="25" t="s">
@@ -9097,7 +9125,7 @@
     </row>
     <row r="210" spans="1:9" ht="30">
       <c r="A210" s="25" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B210" s="26" t="s">
         <v>321</v>
@@ -9110,10 +9138,10 @@
         <v>19</v>
       </c>
       <c r="F210" s="25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G210" s="25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H210" s="25" t="s">
         <v>18</v>
@@ -9122,10 +9150,10 @@
     </row>
     <row r="211" spans="1:9" ht="30">
       <c r="A211" s="25" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B211" s="26" t="s">
-        <v>321</v>
+        <v>625</v>
       </c>
       <c r="C211" s="27" t="s">
         <v>476</v>
@@ -9135,7 +9163,7 @@
         <v>19</v>
       </c>
       <c r="F211" s="25" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G211" s="25" t="s">
         <v>16</v>
@@ -9147,13 +9175,13 @@
     </row>
     <row r="212" spans="1:9" ht="30">
       <c r="A212" s="25" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B212" s="26" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="C212" s="27" t="s">
-        <v>477</v>
+        <v>626</v>
       </c>
       <c r="D212" s="25"/>
       <c r="E212" s="25" t="s">
@@ -9170,37 +9198,37 @@
       </c>
       <c r="I212" s="27"/>
     </row>
-    <row r="213" spans="1:9" ht="30">
+    <row r="213" spans="1:9" ht="165">
       <c r="A213" s="25" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B213" s="26" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="C213" s="27" t="s">
-        <v>632</v>
+        <v>477</v>
       </c>
       <c r="D213" s="25"/>
       <c r="E213" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F213" s="25" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G213" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H213" s="25" t="s">
         <v>18</v>
       </c>
       <c r="I213" s="27"/>
     </row>
-    <row r="214" spans="1:9" ht="165">
+    <row r="214" spans="1:9" ht="45">
       <c r="A214" s="25" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B214" s="26" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
       <c r="C214" s="27" t="s">
         <v>478</v>
@@ -9210,10 +9238,10 @@
         <v>19</v>
       </c>
       <c r="F214" s="25" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G214" s="25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H214" s="25" t="s">
         <v>18</v>
@@ -9222,10 +9250,10 @@
     </row>
     <row r="215" spans="1:9" ht="45">
       <c r="A215" s="25" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B215" s="26" t="s">
-        <v>633</v>
+        <v>322</v>
       </c>
       <c r="C215" s="27" t="s">
         <v>479</v>
@@ -9238,16 +9266,16 @@
         <v>3</v>
       </c>
       <c r="G215" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H215" s="25" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I215" s="27"/>
     </row>
     <row r="216" spans="1:9" ht="45">
       <c r="A216" s="25" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B216" s="26" t="s">
         <v>322</v>
@@ -9270,12 +9298,12 @@
       </c>
       <c r="I216" s="27"/>
     </row>
-    <row r="217" spans="1:9" ht="45">
+    <row r="217" spans="1:9" ht="30">
       <c r="A217" s="25" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B217" s="26" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C217" s="27" t="s">
         <v>481</v>
@@ -9288,16 +9316,16 @@
         <v>3</v>
       </c>
       <c r="G217" s="25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H217" s="25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I217" s="27"/>
     </row>
-    <row r="218" spans="1:9" ht="30">
+    <row r="218" spans="1:9" ht="75">
       <c r="A218" s="25" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B218" s="26" t="s">
         <v>323</v>
@@ -9313,16 +9341,16 @@
         <v>3</v>
       </c>
       <c r="G218" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H218" s="25" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I218" s="27"/>
     </row>
-    <row r="219" spans="1:9" ht="75">
+    <row r="219" spans="1:9" ht="240">
       <c r="A219" s="25" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B219" s="26" t="s">
         <v>323</v>
@@ -9345,9 +9373,9 @@
       </c>
       <c r="I219" s="27"/>
     </row>
-    <row r="220" spans="1:9" ht="240">
+    <row r="220" spans="1:9" ht="30">
       <c r="A220" s="25" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B220" s="26" t="s">
         <v>323</v>
@@ -9360,19 +9388,19 @@
         <v>19</v>
       </c>
       <c r="F220" s="25" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G220" s="25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H220" s="25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I220" s="27"/>
     </row>
-    <row r="221" spans="1:9" ht="30">
+    <row r="221" spans="1:9" ht="90">
       <c r="A221" s="25" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B221" s="26" t="s">
         <v>323</v>
@@ -9388,16 +9416,16 @@
         <v>7</v>
       </c>
       <c r="G221" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H221" s="25" t="s">
         <v>18</v>
       </c>
       <c r="I221" s="27"/>
     </row>
-    <row r="222" spans="1:9" ht="90">
+    <row r="222" spans="1:9" ht="30">
       <c r="A222" s="25" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B222" s="26" t="s">
         <v>323</v>
@@ -9410,25 +9438,25 @@
         <v>19</v>
       </c>
       <c r="F222" s="25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G222" s="25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H222" s="25" t="s">
         <v>18</v>
       </c>
       <c r="I222" s="27"/>
     </row>
-    <row r="223" spans="1:9" ht="30">
+    <row r="223" spans="1:9" ht="60">
       <c r="A223" s="25" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B223" s="26" t="s">
         <v>323</v>
       </c>
-      <c r="C223" s="27" t="s">
-        <v>487</v>
+      <c r="C223" s="16" t="s">
+        <v>642</v>
       </c>
       <c r="D223" s="25"/>
       <c r="E223" s="25" t="s">
@@ -9438,41 +9466,41 @@
         <v>6</v>
       </c>
       <c r="G223" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H223" s="25" t="s">
         <v>18</v>
       </c>
       <c r="I223" s="27"/>
     </row>
-    <row r="224" spans="1:9" ht="45">
+    <row r="224" spans="1:9" ht="30">
       <c r="A224" s="25" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B224" s="26" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C224" s="27" t="s">
-        <v>634</v>
+        <v>487</v>
       </c>
       <c r="D224" s="25"/>
       <c r="E224" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F224" s="25" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G224" s="25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H224" s="25" t="s">
         <v>18</v>
       </c>
       <c r="I224" s="27"/>
     </row>
-    <row r="225" spans="1:9" ht="30">
+    <row r="225" spans="1:9" ht="75">
       <c r="A225" s="25" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B225" s="26" t="s">
         <v>324</v>
@@ -9488,16 +9516,16 @@
         <v>3</v>
       </c>
       <c r="G225" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H225" s="25" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I225" s="27"/>
     </row>
-    <row r="226" spans="1:9" ht="75">
+    <row r="226" spans="1:9" ht="240">
       <c r="A226" s="25" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B226" s="26" t="s">
         <v>324</v>
@@ -9520,9 +9548,9 @@
       </c>
       <c r="I226" s="27"/>
     </row>
-    <row r="227" spans="1:9" ht="240">
+    <row r="227" spans="1:9" ht="30">
       <c r="A227" s="25" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B227" s="26" t="s">
         <v>324</v>
@@ -9535,25 +9563,25 @@
         <v>19</v>
       </c>
       <c r="F227" s="25" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G227" s="25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H227" s="25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I227" s="27"/>
     </row>
-    <row r="228" spans="1:9" ht="30">
+    <row r="228" spans="1:9" ht="75">
       <c r="A228" s="25" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B228" s="26" t="s">
         <v>324</v>
       </c>
       <c r="C228" s="27" t="s">
-        <v>491</v>
+        <v>629</v>
       </c>
       <c r="D228" s="25"/>
       <c r="E228" s="25" t="s">
@@ -9563,22 +9591,22 @@
         <v>7</v>
       </c>
       <c r="G228" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H228" s="25" t="s">
         <v>18</v>
       </c>
       <c r="I228" s="27"/>
     </row>
-    <row r="229" spans="1:9" ht="75">
+    <row r="229" spans="1:9" ht="30">
       <c r="A229" s="25" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B229" s="26" t="s">
         <v>324</v>
       </c>
       <c r="C229" s="27" t="s">
-        <v>638</v>
+        <v>628</v>
       </c>
       <c r="D229" s="25"/>
       <c r="E229" s="25" t="s">
@@ -9597,23 +9625,23 @@
     </row>
     <row r="230" spans="1:9" ht="30">
       <c r="A230" s="25" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B230" s="26" t="s">
         <v>324</v>
       </c>
       <c r="C230" s="27" t="s">
-        <v>637</v>
+        <v>491</v>
       </c>
       <c r="D230" s="25"/>
       <c r="E230" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F230" s="25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G230" s="25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H230" s="25" t="s">
         <v>18</v>
@@ -9622,10 +9650,10 @@
     </row>
     <row r="231" spans="1:9" ht="30">
       <c r="A231" s="25" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B231" s="26" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C231" s="27" t="s">
         <v>492</v>
@@ -9635,7 +9663,7 @@
         <v>19</v>
       </c>
       <c r="F231" s="25" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G231" s="25" t="s">
         <v>16</v>
@@ -9645,9 +9673,9 @@
       </c>
       <c r="I231" s="27"/>
     </row>
-    <row r="232" spans="1:9" ht="30">
+    <row r="232" spans="1:9" ht="75">
       <c r="A232" s="25" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B232" s="26" t="s">
         <v>325</v>
@@ -9663,16 +9691,16 @@
         <v>3</v>
       </c>
       <c r="G232" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H232" s="25" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I232" s="27"/>
     </row>
-    <row r="233" spans="1:9" ht="75">
+    <row r="233" spans="1:9" ht="255">
       <c r="A233" s="25" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B233" s="26" t="s">
         <v>325</v>
@@ -9695,9 +9723,9 @@
       </c>
       <c r="I233" s="27"/>
     </row>
-    <row r="234" spans="1:9" ht="255">
+    <row r="234" spans="1:9" ht="30">
       <c r="A234" s="25" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B234" s="26" t="s">
         <v>325</v>
@@ -9710,19 +9738,19 @@
         <v>19</v>
       </c>
       <c r="F234" s="25" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G234" s="25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H234" s="25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I234" s="27"/>
     </row>
     <row r="235" spans="1:9" ht="30">
       <c r="A235" s="25" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B235" s="26" t="s">
         <v>325</v>
@@ -9735,7 +9763,7 @@
         <v>19</v>
       </c>
       <c r="F235" s="25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G235" s="25" t="s">
         <v>16</v>
@@ -9745,22 +9773,22 @@
       </c>
       <c r="I235" s="27"/>
     </row>
-    <row r="236" spans="1:9" ht="30">
+    <row r="236" spans="1:9" ht="45">
       <c r="A236" s="25" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B236" s="26" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C236" s="27" t="s">
         <v>497</v>
       </c>
       <c r="D236" s="25"/>
       <c r="E236" s="25" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F236" s="25" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G236" s="25" t="s">
         <v>16</v>
@@ -9770,9 +9798,9 @@
       </c>
       <c r="I236" s="27"/>
     </row>
-    <row r="237" spans="1:9" ht="45">
+    <row r="237" spans="1:9" ht="30">
       <c r="A237" s="25" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B237" s="26" t="s">
         <v>326</v>
@@ -9795,9 +9823,9 @@
       </c>
       <c r="I237" s="27"/>
     </row>
-    <row r="238" spans="1:9" ht="30">
+    <row r="238" spans="1:9" ht="45">
       <c r="A238" s="25" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B238" s="26" t="s">
         <v>326</v>
@@ -9805,7 +9833,9 @@
       <c r="C238" s="27" t="s">
         <v>499</v>
       </c>
-      <c r="D238" s="25"/>
+      <c r="D238" s="25" t="s">
+        <v>549</v>
+      </c>
       <c r="E238" s="25" t="s">
         <v>22</v>
       </c>
@@ -9813,25 +9843,27 @@
         <v>3</v>
       </c>
       <c r="G238" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H238" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="I238" s="27"/>
+        <v>21</v>
+      </c>
+      <c r="I238" s="27" t="s">
+        <v>552</v>
+      </c>
     </row>
     <row r="239" spans="1:9" ht="45">
       <c r="A239" s="25" t="s">
-        <v>244</v>
+        <v>562</v>
       </c>
       <c r="B239" s="26" t="s">
         <v>326</v>
       </c>
       <c r="C239" s="27" t="s">
-        <v>500</v>
+        <v>565</v>
       </c>
       <c r="D239" s="25" t="s">
-        <v>550</v>
+        <v>563</v>
       </c>
       <c r="E239" s="25" t="s">
         <v>22</v>
@@ -9846,24 +9878,22 @@
         <v>21</v>
       </c>
       <c r="I239" s="27" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="240" spans="1:9" ht="45">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="240" spans="1:9" ht="165">
       <c r="A240" s="25" t="s">
-        <v>563</v>
+        <v>245</v>
       </c>
       <c r="B240" s="26" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C240" s="27" t="s">
-        <v>566</v>
-      </c>
-      <c r="D240" s="25" t="s">
-        <v>564</v>
-      </c>
+        <v>500</v>
+      </c>
+      <c r="D240" s="25"/>
       <c r="E240" s="25" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F240" s="25" t="s">
         <v>3</v>
@@ -9874,16 +9904,14 @@
       <c r="H240" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="I240" s="27" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="241" spans="1:9" ht="165">
+      <c r="I240" s="27"/>
+    </row>
+    <row r="241" spans="1:9" ht="225">
       <c r="A241" s="25" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B241" s="26" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C241" s="27" t="s">
         <v>501</v>
@@ -9903,9 +9931,9 @@
       </c>
       <c r="I241" s="27"/>
     </row>
-    <row r="242" spans="1:9" ht="225">
+    <row r="242" spans="1:9" ht="30">
       <c r="A242" s="25" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B242" s="26" t="s">
         <v>328</v>
@@ -9930,7 +9958,7 @@
     </row>
     <row r="243" spans="1:9" ht="30">
       <c r="A243" s="25" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B243" s="26" t="s">
         <v>328</v>
@@ -9955,7 +9983,7 @@
     </row>
     <row r="244" spans="1:9" ht="30">
       <c r="A244" s="25" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B244" s="26" t="s">
         <v>328</v>
@@ -9980,13 +10008,13 @@
     </row>
     <row r="245" spans="1:9" ht="30">
       <c r="A245" s="25" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B245" s="26" t="s">
         <v>328</v>
       </c>
       <c r="C245" s="27" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D245" s="25"/>
       <c r="E245" s="25" t="s">
@@ -10003,12 +10031,12 @@
       </c>
       <c r="I245" s="27"/>
     </row>
-    <row r="246" spans="1:9" ht="30">
+    <row r="246" spans="1:9" ht="90">
       <c r="A246" s="25" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B246" s="26" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C246" s="27" t="s">
         <v>505</v>
@@ -10028,9 +10056,9 @@
       </c>
       <c r="I246" s="27"/>
     </row>
-    <row r="247" spans="1:9" ht="90">
+    <row r="247" spans="1:9" ht="60">
       <c r="A247" s="25" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B247" s="26" t="s">
         <v>329</v>
@@ -10053,12 +10081,12 @@
       </c>
       <c r="I247" s="27"/>
     </row>
-    <row r="248" spans="1:9" ht="60">
+    <row r="248" spans="1:9" ht="409.5">
       <c r="A248" s="25" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B248" s="26" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C248" s="27" t="s">
         <v>507</v>
@@ -10078,12 +10106,12 @@
       </c>
       <c r="I248" s="27"/>
     </row>
-    <row r="249" spans="1:9" ht="409.5">
+    <row r="249" spans="1:9" ht="225">
       <c r="A249" s="25" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B249" s="26" t="s">
-        <v>330</v>
+        <v>32</v>
       </c>
       <c r="C249" s="27" t="s">
         <v>508</v>
@@ -10099,13 +10127,13 @@
         <v>15</v>
       </c>
       <c r="H249" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I249" s="27"/>
     </row>
-    <row r="250" spans="1:9" ht="225">
+    <row r="250" spans="1:9" ht="30">
       <c r="A250" s="25" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B250" s="26" t="s">
         <v>32</v>
@@ -10128,12 +10156,12 @@
       </c>
       <c r="I250" s="27"/>
     </row>
-    <row r="251" spans="1:9" ht="30">
+    <row r="251" spans="1:9" ht="270">
       <c r="A251" s="25" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B251" s="26" t="s">
-        <v>32</v>
+        <v>303</v>
       </c>
       <c r="C251" s="27" t="s">
         <v>510</v>
@@ -10153,9 +10181,9 @@
       </c>
       <c r="I251" s="27"/>
     </row>
-    <row r="252" spans="1:9" ht="270">
+    <row r="252" spans="1:9" ht="30">
       <c r="A252" s="25" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B252" s="26" t="s">
         <v>303</v>
@@ -10180,7 +10208,7 @@
     </row>
     <row r="253" spans="1:9" ht="30">
       <c r="A253" s="25" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B253" s="26" t="s">
         <v>303</v>
@@ -10203,12 +10231,12 @@
       </c>
       <c r="I253" s="27"/>
     </row>
-    <row r="254" spans="1:9" ht="30">
+    <row r="254" spans="1:9" ht="150">
       <c r="A254" s="25" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B254" s="26" t="s">
-        <v>303</v>
+        <v>331</v>
       </c>
       <c r="C254" s="27" t="s">
         <v>513</v>
@@ -10224,16 +10252,16 @@
         <v>15</v>
       </c>
       <c r="H254" s="25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I254" s="27"/>
     </row>
-    <row r="255" spans="1:9" ht="150">
+    <row r="255" spans="1:9" ht="135">
       <c r="A255" s="25" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B255" s="26" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C255" s="27" t="s">
         <v>514</v>
@@ -10249,16 +10277,16 @@
         <v>15</v>
       </c>
       <c r="H255" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I255" s="27"/>
     </row>
-    <row r="256" spans="1:9" ht="135">
+    <row r="256" spans="1:9" ht="225">
       <c r="A256" s="25" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B256" s="26" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C256" s="27" t="s">
         <v>515</v>
@@ -10274,16 +10302,16 @@
         <v>15</v>
       </c>
       <c r="H256" s="25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I256" s="27"/>
     </row>
-    <row r="257" spans="1:9" ht="225">
+    <row r="257" spans="1:9" ht="255">
       <c r="A257" s="25" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B257" s="26" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C257" s="27" t="s">
         <v>516</v>
@@ -10303,9 +10331,9 @@
       </c>
       <c r="I257" s="27"/>
     </row>
-    <row r="258" spans="1:9" ht="255">
+    <row r="258" spans="1:9" ht="30">
       <c r="A258" s="25" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B258" s="26" t="s">
         <v>334</v>
@@ -10330,7 +10358,7 @@
     </row>
     <row r="259" spans="1:9" ht="30">
       <c r="A259" s="25" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B259" s="26" t="s">
         <v>334</v>
@@ -10349,16 +10377,16 @@
         <v>15</v>
       </c>
       <c r="H259" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I259" s="27"/>
     </row>
-    <row r="260" spans="1:9" ht="30">
+    <row r="260" spans="1:9" ht="135">
       <c r="A260" s="25" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B260" s="26" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C260" s="27" t="s">
         <v>519</v>
@@ -10374,16 +10402,16 @@
         <v>15</v>
       </c>
       <c r="H260" s="25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I260" s="27"/>
     </row>
-    <row r="261" spans="1:9" ht="135">
+    <row r="261" spans="1:9" ht="225">
       <c r="A261" s="25" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B261" s="26" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C261" s="27" t="s">
         <v>520</v>
@@ -10403,12 +10431,12 @@
       </c>
       <c r="I261" s="27"/>
     </row>
-    <row r="262" spans="1:9" ht="225">
+    <row r="262" spans="1:9" ht="270">
       <c r="A262" s="25" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B262" s="26" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C262" s="27" t="s">
         <v>521</v>
@@ -10424,13 +10452,13 @@
         <v>15</v>
       </c>
       <c r="H262" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I262" s="27"/>
     </row>
-    <row r="263" spans="1:9" ht="270">
+    <row r="263" spans="1:9" ht="30">
       <c r="A263" s="25" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B263" s="26" t="s">
         <v>337</v>
@@ -10449,13 +10477,13 @@
         <v>15</v>
       </c>
       <c r="H263" s="25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I263" s="27"/>
     </row>
-    <row r="264" spans="1:9" ht="30">
+    <row r="264" spans="1:9" ht="45">
       <c r="A264" s="25" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B264" s="26" t="s">
         <v>337</v>
@@ -10474,13 +10502,13 @@
         <v>15</v>
       </c>
       <c r="H264" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I264" s="27"/>
     </row>
-    <row r="265" spans="1:9" ht="45">
+    <row r="265" spans="1:9" ht="30">
       <c r="A265" s="25" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B265" s="26" t="s">
         <v>337</v>
@@ -10499,13 +10527,13 @@
         <v>15</v>
       </c>
       <c r="H265" s="25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I265" s="27"/>
     </row>
-    <row r="266" spans="1:9" ht="30">
+    <row r="266" spans="1:9" ht="45">
       <c r="A266" s="25" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B266" s="26" t="s">
         <v>337</v>
@@ -10524,16 +10552,16 @@
         <v>15</v>
       </c>
       <c r="H266" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I266" s="27"/>
     </row>
-    <row r="267" spans="1:9" ht="45">
+    <row r="267" spans="1:9" ht="315">
       <c r="A267" s="25" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B267" s="26" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C267" s="27" t="s">
         <v>526</v>
@@ -10553,9 +10581,9 @@
       </c>
       <c r="I267" s="27"/>
     </row>
-    <row r="268" spans="1:9" ht="315">
+    <row r="268" spans="1:9" ht="30">
       <c r="A268" s="25" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B268" s="26" t="s">
         <v>338</v>
@@ -10574,19 +10602,19 @@
         <v>15</v>
       </c>
       <c r="H268" s="25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I268" s="27"/>
     </row>
-    <row r="269" spans="1:9" ht="30">
+    <row r="269" spans="1:9" ht="45">
       <c r="A269" s="25" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B269" s="26" t="s">
-        <v>338</v>
+        <v>633</v>
       </c>
       <c r="C269" s="27" t="s">
-        <v>528</v>
+        <v>634</v>
       </c>
       <c r="D269" s="25"/>
       <c r="E269" s="25" t="s">
@@ -10599,19 +10627,19 @@
         <v>15</v>
       </c>
       <c r="H269" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I269" s="27"/>
     </row>
-    <row r="270" spans="1:9" ht="45">
+    <row r="270" spans="1:9" ht="30">
       <c r="A270" s="25" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B270" s="26" t="s">
-        <v>643</v>
+        <v>633</v>
       </c>
       <c r="C270" s="27" t="s">
-        <v>644</v>
+        <v>528</v>
       </c>
       <c r="D270" s="25"/>
       <c r="E270" s="25" t="s">
@@ -10630,10 +10658,10 @@
     </row>
     <row r="271" spans="1:9" ht="30">
       <c r="A271" s="25" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B271" s="26" t="s">
-        <v>643</v>
+        <v>338</v>
       </c>
       <c r="C271" s="27" t="s">
         <v>529</v>
@@ -10649,19 +10677,19 @@
         <v>15</v>
       </c>
       <c r="H271" s="25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I271" s="27"/>
     </row>
-    <row r="272" spans="1:9" ht="30">
+    <row r="272" spans="1:9" ht="45">
       <c r="A272" s="25" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B272" s="26" t="s">
-        <v>338</v>
+        <v>633</v>
       </c>
       <c r="C272" s="27" t="s">
-        <v>530</v>
+        <v>635</v>
       </c>
       <c r="D272" s="25"/>
       <c r="E272" s="25" t="s">
@@ -10674,19 +10702,19 @@
         <v>15</v>
       </c>
       <c r="H272" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I272" s="27"/>
     </row>
-    <row r="273" spans="1:9" ht="45">
+    <row r="273" spans="1:9" ht="30">
       <c r="A273" s="25" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B273" s="26" t="s">
-        <v>643</v>
+        <v>338</v>
       </c>
       <c r="C273" s="27" t="s">
-        <v>645</v>
+        <v>530</v>
       </c>
       <c r="D273" s="25"/>
       <c r="E273" s="25" t="s">
@@ -10705,7 +10733,7 @@
     </row>
     <row r="274" spans="1:9" ht="30">
       <c r="A274" s="25" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B274" s="26" t="s">
         <v>338</v>
@@ -10724,13 +10752,13 @@
         <v>15</v>
       </c>
       <c r="H274" s="25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I274" s="27"/>
     </row>
     <row r="275" spans="1:9" ht="30">
       <c r="A275" s="25" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B275" s="26" t="s">
         <v>338</v>
@@ -10749,13 +10777,13 @@
         <v>15</v>
       </c>
       <c r="H275" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I275" s="27"/>
     </row>
     <row r="276" spans="1:9" ht="30">
       <c r="A276" s="25" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B276" s="26" t="s">
         <v>338</v>
@@ -10778,12 +10806,12 @@
       </c>
       <c r="I276" s="27"/>
     </row>
-    <row r="277" spans="1:9" ht="30">
+    <row r="277" spans="1:9" ht="285">
       <c r="A277" s="25" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B277" s="26" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C277" s="27" t="s">
         <v>534</v>
@@ -10803,9 +10831,9 @@
       </c>
       <c r="I277" s="27"/>
     </row>
-    <row r="278" spans="1:9" ht="285">
+    <row r="278" spans="1:9" ht="30">
       <c r="A278" s="25" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B278" s="26" t="s">
         <v>339</v>
@@ -10824,13 +10852,13 @@
         <v>15</v>
       </c>
       <c r="H278" s="25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I278" s="27"/>
     </row>
-    <row r="279" spans="1:9" ht="30">
+    <row r="279" spans="1:9" ht="45">
       <c r="A279" s="25" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B279" s="26" t="s">
         <v>339</v>
@@ -10849,13 +10877,13 @@
         <v>15</v>
       </c>
       <c r="H279" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I279" s="27"/>
     </row>
-    <row r="280" spans="1:9" ht="45">
+    <row r="280" spans="1:9" ht="60">
       <c r="A280" s="25" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B280" s="26" t="s">
         <v>339</v>
@@ -10874,16 +10902,18 @@
         <v>15</v>
       </c>
       <c r="H280" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="I280" s="27"/>
-    </row>
-    <row r="281" spans="1:9" ht="60">
+        <v>17</v>
+      </c>
+      <c r="I280" s="27" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="281" spans="1:9" ht="255">
       <c r="A281" s="25" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B281" s="26" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C281" s="27" t="s">
         <v>538</v>
@@ -10899,15 +10929,13 @@
         <v>15</v>
       </c>
       <c r="H281" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="I281" s="27" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="282" spans="1:9" ht="255">
+        <v>21</v>
+      </c>
+      <c r="I281" s="27"/>
+    </row>
+    <row r="282" spans="1:9" ht="30">
       <c r="A282" s="25" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B282" s="26" t="s">
         <v>340</v>
@@ -10930,9 +10958,9 @@
       </c>
       <c r="I282" s="27"/>
     </row>
-    <row r="283" spans="1:9" ht="30">
+    <row r="283" spans="1:9" ht="45">
       <c r="A283" s="25" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B283" s="26" t="s">
         <v>340</v>
@@ -10951,13 +10979,13 @@
         <v>15</v>
       </c>
       <c r="H283" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I283" s="27"/>
     </row>
-    <row r="284" spans="1:9" ht="45">
+    <row r="284" spans="1:9" ht="30">
       <c r="A284" s="25" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B284" s="26" t="s">
         <v>340</v>
@@ -10976,13 +11004,13 @@
         <v>15</v>
       </c>
       <c r="H284" s="25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I284" s="27"/>
     </row>
-    <row r="285" spans="1:9" ht="30">
+    <row r="285" spans="1:9" ht="45">
       <c r="A285" s="25" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B285" s="26" t="s">
         <v>340</v>
@@ -11001,13 +11029,13 @@
         <v>15</v>
       </c>
       <c r="H285" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I285" s="27"/>
     </row>
-    <row r="286" spans="1:9" ht="45">
+    <row r="286" spans="1:9" ht="30">
       <c r="A286" s="25" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B286" s="26" t="s">
         <v>340</v>
@@ -11026,13 +11054,13 @@
         <v>15</v>
       </c>
       <c r="H286" s="25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I286" s="27"/>
     </row>
-    <row r="287" spans="1:9" ht="30">
+    <row r="287" spans="1:9" ht="45">
       <c r="A287" s="25" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B287" s="26" t="s">
         <v>340</v>
@@ -11051,26 +11079,28 @@
         <v>15</v>
       </c>
       <c r="H287" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I287" s="27"/>
     </row>
     <row r="288" spans="1:9" ht="45">
       <c r="A288" s="25" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B288" s="26" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="C288" s="27" t="s">
         <v>545</v>
       </c>
-      <c r="D288" s="25"/>
+      <c r="D288" s="25" t="s">
+        <v>550</v>
+      </c>
       <c r="E288" s="25" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F288" s="25" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G288" s="25" t="s">
         <v>15</v>
@@ -11078,11 +11108,13 @@
       <c r="H288" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="I288" s="27"/>
+      <c r="I288" s="27" t="s">
+        <v>552</v>
+      </c>
     </row>
     <row r="289" spans="1:9" ht="45">
       <c r="A289" s="25" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B289" s="26" t="s">
         <v>326</v>
@@ -11091,7 +11123,7 @@
         <v>546</v>
       </c>
       <c r="D289" s="25" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="E289" s="25" t="s">
         <v>22</v>
@@ -11106,128 +11138,99 @@
         <v>20</v>
       </c>
       <c r="I289" s="27" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="290" spans="1:9" ht="45">
-      <c r="A290" s="25" t="s">
-        <v>294</v>
-      </c>
-      <c r="B290" s="26" t="s">
-        <v>326</v>
-      </c>
-      <c r="C290" s="27" t="s">
-        <v>547</v>
-      </c>
-      <c r="D290" s="25" t="s">
-        <v>551</v>
-      </c>
-      <c r="E290" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="F290" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="G290" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="H290" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="I290" s="27" t="s">
-        <v>553</v>
-      </c>
+        <v>552</v>
+      </c>
+    </row>
+    <row r="290" spans="1:9">
+      <c r="A290" s="3"/>
+      <c r="B290" s="9"/>
     </row>
     <row r="291" spans="1:9">
       <c r="A291" s="3"/>
       <c r="B291" s="9"/>
     </row>
-    <row r="292" spans="1:9">
-      <c r="A292" s="3"/>
-      <c r="B292" s="9"/>
-    </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B8:I8"/>
     <mergeCell ref="B18:I18"/>
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="B16:I16"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B8:I8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A20:H52 A35:I290">
-    <cfRule type="expression" dxfId="30" priority="53">
+  <conditionalFormatting sqref="A20:H52 A35:I289">
+    <cfRule type="expression" dxfId="13" priority="53">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="54">
+    <cfRule type="expression" dxfId="12" priority="54">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="61">
+    <cfRule type="expression" dxfId="11" priority="61">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A20:H52 A35:I290">
-    <cfRule type="expression" dxfId="27" priority="7">
+  <conditionalFormatting sqref="A20:H52 A35:I289">
+    <cfRule type="expression" dxfId="10" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="8">
+    <cfRule type="expression" dxfId="9" priority="8">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="9">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F20:F290">
-    <cfRule type="expression" dxfId="24" priority="13">
+  <conditionalFormatting sqref="F20:F289">
+    <cfRule type="expression" dxfId="7" priority="13">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="14">
+    <cfRule type="expression" dxfId="6" priority="14">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:I52">
-    <cfRule type="expression" dxfId="22" priority="4">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="6">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:I52">
-    <cfRule type="expression" dxfId="19" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 F20:F290">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 F20:F289" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$A$13:$A$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 E20:E290">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 E20:E289" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Protocol,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4 G20:G290">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4 G20:G289" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Informative,Normative"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"In, Out"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H290">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H289" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
   </dataValidations>
@@ -11237,7 +11240,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B1:B9 B10:B16 B240:B271 B18:B136 B143:B215 B137:B142 B216:B239 B272:B273 B274:B292 C3" numberStoredAsText="1"/>
+    <ignoredError sqref="B1:B9 B10:B16 B239:B270 B18:B135 B142:B214 B136:B141 B215:B238 B271:B272 B273:B291" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
@@ -11247,21 +11250,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -11310,16 +11298,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11333,16 +11337,15 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update RS of MS-OXWSTASK.
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSTASK/MS-OXWSTASK_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSTASK/MS-OXWSTASK_RequirementSpecification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-xiahu\Desktop\test suite\Interop-TestSuites-1-master\ExchangeWebServices\Docs\MS-OXWSTASK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D25184-9436-4AFB-9FAB-B6620E2794A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A3DE51-894C-4420-B61B-C605CDA404CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -2499,9 +2499,6 @@
     <t>[In t:TaskType Complex Type] This element [IsAssignmentEditable] is read-only for the client.</t>
   </si>
   <si>
-    <t>[In t:TaskType Complex Type] The type of IsComplete is xs:boolean [XMLSCHEMA2] section 3.2.2.</t>
-  </si>
-  <si>
     <t>MS-OXWSTASK_R5556001</t>
   </si>
   <si>
@@ -2524,9 +2521,6 @@
   </si>
   <si>
     <t>[In t:TaskType Complex Type] Once the task item is created, this property is read-only for the client.&lt;1&gt;</t>
-  </si>
-  <si>
-    <t>[In t:TaskType Complex Type] The type of PercentComplete is xs:double [XMLSCHEMA2] section 3.2.5.</t>
   </si>
   <si>
     <t>[In t:TaskType Complex Type] The type of Recurrence is t:TaskRecurrenceType (section 2.2.4.4).</t>
@@ -2685,16 +2679,22 @@
     <t>[In t:TaskType Complex Type] The type of BillingInformation is xs:string [XMLSCHEMA2/2] section 3.2.1.</t>
   </si>
   <si>
-    <t>[In CopyItem Operation] tns:CopyItemSoapIn([MS-OXWSCORE] section 3.1.4.1.1.1)%5BMS-OXWSCORE%5D.pdf: Specifies the SOAP message that defines the task item to be copied.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[In CopyItem Operation] tns:CopyItemSoapIn ([MS-OXWSCORE] section 3.1.4.1.1.1)%5BMS-OXWSCORE%5D.pdf: The CopyItem operation (as specified in [MS-OXWSCORE] section 3.1.4.1.1.1) that specifies the XML request MUST contain the t:TargetFolderIdType complex type (as specified in [MS-OXWSFOLD] section 2.2.4.16) and the t:ItemIdType complex type (as specified in [MS-OXWSCORE] section 2.2.4.25). </t>
-  </si>
-  <si>
-    <t>[In CopyItem Operation] tns:CopyItemSoapIn ([MS-OXWSCORE] section 3.1.4.1.1.1)%5BMS-OXWSCORE%5D.pdf: All other type elements in t:NonEmptyArrayOfBaseItemIdsType element MUST NOT be included.</t>
-  </si>
-  <si>
     <t>[In GetItem Operation] [tns:GetItemSoapOut ([MS-OXWSCORE] section 3.1.4.4.1.2)] The server returns a  t:GetItemResponseType complex type element, which extends the BaseResponseMessageType complex type, as specified in [MS-OXWSCDATA] section 2.2.4.18, that contains properties associated with the task item.</t>
+  </si>
+  <si>
+    <t>[In t:TaskType Complex Type] The type of IsComplete is xs:boolean [XMLSCHEMA2/2] section 3.2.2.</t>
+  </si>
+  <si>
+    <t>[In t:TaskType Complex Type] The type of PercentComplete is xs:double [XMLSCHEMA2/2] section 3.2.5.</t>
+  </si>
+  <si>
+    <t>[In CopyItem Operation] tns:CopyItemSoapIn([MS-OXWSCORE] section 3.1.4.1.1.1): Specifies the SOAP message that defines the task item to be copied.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[In CopyItem Operation] tns:CopyItemSoapIn ([MS-OXWSCORE] section 3.1.4.1.1.1): The CopyItem operation (as specified in [MS-OXWSCORE] section 3.1.4.1.1.1) that specifies the XML request MUST contain the t:TargetFolderIdType complex type (as specified in [MS-OXWSFOLD] section 2.2.4.16) and the t:ItemIdType complex type (as specified in [MS-OXWSCORE] section 2.2.4.25). </t>
+  </si>
+  <si>
+    <t>[In CopyItem Operation] tns:CopyItemSoapIn ([MS-OXWSCORE] section 3.1.4.1.1.1): All other type elements in t:NonEmptyArrayOfBaseItemIdsType element MUST NOT be included.</t>
   </si>
 </sst>
 </file>
@@ -3045,6 +3045,9 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3102,88 +3105,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="31">
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3503,6 +3429,80 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3632,34 +3632,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I289" tableType="xml" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I289" tableType="xml" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" connectionId="1">
   <autoFilter ref="A19:I289" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="28">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="27">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="26">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="25">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="24">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="23">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="22">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="21">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="7">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="20">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="6">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -3668,12 +3668,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A12:C15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4003,8 +4003,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A220" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C224" sqref="C224"/>
+    <sheetView tabSelected="1" topLeftCell="A202" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C195" sqref="C195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -4053,7 +4053,7 @@
       <c r="B3" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="63">
+      <c r="C3" s="44">
         <v>8.1</v>
       </c>
       <c r="D3" s="4"/>
@@ -4070,16 +4070,16 @@
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" ht="21">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
       <c r="I4" s="32"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -4091,13 +4091,13 @@
       <c r="B5" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="56"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="57"/>
-      <c r="I5" s="58"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="59"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
@@ -4105,16 +4105,16 @@
       <c r="A6" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="58"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="59"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
@@ -4122,16 +4122,16 @@
       <c r="A7" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="60" t="s">
+      <c r="B7" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="61"/>
-      <c r="H7" s="61"/>
-      <c r="I7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="63"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
@@ -4139,16 +4139,16 @@
       <c r="A8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="60" t="s">
+      <c r="B8" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="62"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="63"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
@@ -4156,16 +4156,16 @@
       <c r="A9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="50"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
     </row>
@@ -4173,16 +4173,16 @@
       <c r="A10" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="48"/>
-      <c r="I10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="50"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
     </row>
@@ -4190,16 +4190,16 @@
       <c r="A11" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="51" t="s">
         <v>556</v>
       </c>
-      <c r="C11" s="51"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="46"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="47"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
     </row>
@@ -4283,16 +4283,16 @@
       <c r="A16" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="52" t="s">
+      <c r="B16" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="53"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="46"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="47"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
     </row>
@@ -4300,16 +4300,16 @@
       <c r="A17" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="55" t="s">
         <v>558</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="46"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="47"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
     </row>
@@ -4317,16 +4317,16 @@
       <c r="A18" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="44" t="s">
+      <c r="B18" s="45" t="s">
         <v>557</v>
       </c>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="46"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="47"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="M18" s="4"/>
@@ -5573,7 +5573,7 @@
         <v>307</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="D68" s="25"/>
       <c r="E68" s="25" t="s">
@@ -5623,7 +5623,7 @@
         <v>307</v>
       </c>
       <c r="C70" s="16" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="D70" s="25"/>
       <c r="E70" s="25" t="s">
@@ -5673,7 +5673,7 @@
         <v>307</v>
       </c>
       <c r="C72" s="16" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="D72" s="25"/>
       <c r="E72" s="25" t="s">
@@ -5748,7 +5748,7 @@
         <v>307</v>
       </c>
       <c r="C75" s="27" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="D75" s="25"/>
       <c r="E75" s="25" t="s">
@@ -5767,13 +5767,13 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" s="25" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B76" s="26" t="s">
         <v>307</v>
       </c>
       <c r="C76" s="27" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="D76" s="25"/>
       <c r="E76" s="25" t="s">
@@ -6122,8 +6122,8 @@
       <c r="B90" s="26" t="s">
         <v>307</v>
       </c>
-      <c r="C90" s="27" t="s">
-        <v>581</v>
+      <c r="C90" s="16" t="s">
+        <v>638</v>
       </c>
       <c r="D90" s="25"/>
       <c r="E90" s="25" t="s">
@@ -6221,13 +6221,13 @@
     </row>
     <row r="94" spans="1:9">
       <c r="A94" s="25" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B94" s="26" t="s">
         <v>307</v>
       </c>
       <c r="C94" s="27" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D94" s="25"/>
       <c r="E94" s="25" t="s">
@@ -6350,13 +6350,13 @@
     </row>
     <row r="99" spans="1:9">
       <c r="A99" s="25" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B99" s="26" t="s">
         <v>307</v>
       </c>
       <c r="C99" s="27" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D99" s="25"/>
       <c r="E99" s="25" t="s">
@@ -6400,13 +6400,13 @@
     </row>
     <row r="101" spans="1:9">
       <c r="A101" s="25" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B101" s="26" t="s">
         <v>307</v>
       </c>
       <c r="C101" s="27" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D101" s="25"/>
       <c r="E101" s="25" t="s">
@@ -6500,13 +6500,13 @@
     </row>
     <row r="105" spans="1:9" ht="30">
       <c r="A105" s="25" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B105" s="26" t="s">
         <v>307</v>
       </c>
       <c r="C105" s="27" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D105" s="25"/>
       <c r="E105" s="25" t="s">
@@ -6530,8 +6530,8 @@
       <c r="B106" s="26" t="s">
         <v>307</v>
       </c>
-      <c r="C106" s="27" t="s">
-        <v>590</v>
+      <c r="C106" s="16" t="s">
+        <v>639</v>
       </c>
       <c r="D106" s="25"/>
       <c r="E106" s="25" t="s">
@@ -6581,7 +6581,7 @@
         <v>307</v>
       </c>
       <c r="C108" s="27" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="D108" s="25"/>
       <c r="E108" s="25" t="s">
@@ -6775,13 +6775,13 @@
     </row>
     <row r="116" spans="1:9">
       <c r="A116" s="25" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="B116" s="26" t="s">
         <v>307</v>
       </c>
       <c r="C116" s="27" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="D116" s="25"/>
       <c r="E116" s="25" t="s">
@@ -6850,13 +6850,13 @@
     </row>
     <row r="119" spans="1:9" ht="30">
       <c r="A119" s="25" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="B119" s="26" t="s">
         <v>307</v>
       </c>
       <c r="C119" s="27" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="D119" s="25"/>
       <c r="E119" s="25" t="s">
@@ -6875,13 +6875,13 @@
     </row>
     <row r="120" spans="1:9" ht="30">
       <c r="A120" s="25" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="B120" s="26" t="s">
         <v>307</v>
       </c>
       <c r="C120" s="27" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D120" s="25"/>
       <c r="E120" s="25" t="s">
@@ -6900,13 +6900,13 @@
     </row>
     <row r="121" spans="1:9" ht="60">
       <c r="A121" s="25" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="B121" s="26" t="s">
         <v>307</v>
       </c>
       <c r="C121" s="27" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="D121" s="25"/>
       <c r="E121" s="25" t="s">
@@ -6956,7 +6956,7 @@
         <v>308</v>
       </c>
       <c r="C123" s="27" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="D123" s="25"/>
       <c r="E123" s="25" t="s">
@@ -7006,7 +7006,7 @@
         <v>309</v>
       </c>
       <c r="C125" s="27" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="D125" s="25"/>
       <c r="E125" s="25" t="s">
@@ -7256,7 +7256,7 @@
         <v>311</v>
       </c>
       <c r="C135" s="27" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="D135" s="25"/>
       <c r="E135" s="25" t="s">
@@ -7281,7 +7281,7 @@
         <v>311</v>
       </c>
       <c r="C136" s="27" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="D136" s="25"/>
       <c r="E136" s="25" t="s">
@@ -7331,7 +7331,7 @@
         <v>311</v>
       </c>
       <c r="C138" s="27" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="D138" s="25"/>
       <c r="E138" s="25" t="s">
@@ -7356,7 +7356,7 @@
         <v>311</v>
       </c>
       <c r="C139" s="27" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="D139" s="25"/>
       <c r="E139" s="25" t="s">
@@ -7381,7 +7381,7 @@
         <v>311</v>
       </c>
       <c r="C140" s="27" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="D140" s="25"/>
       <c r="E140" s="25" t="s">
@@ -7400,13 +7400,13 @@
     </row>
     <row r="141" spans="1:9" ht="30">
       <c r="A141" s="25" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B141" s="26" t="s">
         <v>311</v>
       </c>
       <c r="C141" s="27" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="D141" s="25"/>
       <c r="E141" s="25" t="s">
@@ -7425,13 +7425,13 @@
     </row>
     <row r="142" spans="1:9" ht="45">
       <c r="A142" s="25" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="B142" s="26" t="s">
         <v>311</v>
       </c>
       <c r="C142" s="27" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="D142" s="25"/>
       <c r="E142" s="25" t="s">
@@ -7781,7 +7781,7 @@
         <v>315</v>
       </c>
       <c r="C156" s="27" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="D156" s="25"/>
       <c r="E156" s="25" t="s">
@@ -7881,7 +7881,7 @@
         <v>315</v>
       </c>
       <c r="C160" s="27" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="D160" s="25"/>
       <c r="E160" s="25" t="s">
@@ -7981,7 +7981,7 @@
         <v>315</v>
       </c>
       <c r="C164" s="27" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="D164" s="25"/>
       <c r="E164" s="25" t="s">
@@ -8031,7 +8031,7 @@
         <v>315</v>
       </c>
       <c r="C166" s="27" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="D166" s="25"/>
       <c r="E166" s="25" t="s">
@@ -8081,7 +8081,7 @@
         <v>315</v>
       </c>
       <c r="C168" s="27" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="D168" s="25"/>
       <c r="E168" s="25" t="s">
@@ -8181,7 +8181,7 @@
         <v>315</v>
       </c>
       <c r="C172" s="27" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="D172" s="25"/>
       <c r="E172" s="25" t="s">
@@ -8481,7 +8481,7 @@
         <v>320</v>
       </c>
       <c r="C184" s="27" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="D184" s="25"/>
       <c r="E184" s="25" t="s">
@@ -8506,7 +8506,7 @@
         <v>320</v>
       </c>
       <c r="C185" s="27" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="D185" s="25"/>
       <c r="E185" s="25" t="s">
@@ -8531,7 +8531,7 @@
         <v>320</v>
       </c>
       <c r="C186" s="27" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="D186" s="25"/>
       <c r="E186" s="25" t="s">
@@ -8556,7 +8556,7 @@
         <v>320</v>
       </c>
       <c r="C187" s="27" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="D187" s="25"/>
       <c r="E187" s="25" t="s">
@@ -8581,7 +8581,7 @@
         <v>320</v>
       </c>
       <c r="C188" s="27" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="D188" s="25"/>
       <c r="E188" s="25" t="s">
@@ -8606,7 +8606,7 @@
         <v>320</v>
       </c>
       <c r="C189" s="27" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="D189" s="25"/>
       <c r="E189" s="25" t="s">
@@ -8706,7 +8706,7 @@
         <v>33</v>
       </c>
       <c r="C193" s="16" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="D193" s="25"/>
       <c r="E193" s="25" t="s">
@@ -8731,7 +8731,7 @@
         <v>33</v>
       </c>
       <c r="C194" s="16" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="D194" s="25"/>
       <c r="E194" s="25" t="s">
@@ -8756,7 +8756,7 @@
         <v>33</v>
       </c>
       <c r="C195" s="16" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="D195" s="25"/>
       <c r="E195" s="25" t="s">
@@ -8906,7 +8906,7 @@
         <v>34</v>
       </c>
       <c r="C201" s="27" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="D201" s="25"/>
       <c r="E201" s="25" t="s">
@@ -9081,7 +9081,7 @@
         <v>321</v>
       </c>
       <c r="C208" s="27" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="D208" s="25"/>
       <c r="E208" s="25" t="s">
@@ -9153,7 +9153,7 @@
         <v>217</v>
       </c>
       <c r="B211" s="26" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="C211" s="27" t="s">
         <v>476</v>
@@ -9178,10 +9178,10 @@
         <v>218</v>
       </c>
       <c r="B212" s="26" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="C212" s="27" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="D212" s="25"/>
       <c r="E212" s="25" t="s">
@@ -9203,7 +9203,7 @@
         <v>219</v>
       </c>
       <c r="B213" s="26" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="C213" s="27" t="s">
         <v>477</v>
@@ -9228,7 +9228,7 @@
         <v>220</v>
       </c>
       <c r="B214" s="26" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="C214" s="27" t="s">
         <v>478</v>
@@ -9456,7 +9456,7 @@
         <v>323</v>
       </c>
       <c r="C223" s="16" t="s">
-        <v>642</v>
+        <v>637</v>
       </c>
       <c r="D223" s="25"/>
       <c r="E223" s="25" t="s">
@@ -9581,7 +9581,7 @@
         <v>324</v>
       </c>
       <c r="C228" s="27" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="D228" s="25"/>
       <c r="E228" s="25" t="s">
@@ -9606,7 +9606,7 @@
         <v>324</v>
       </c>
       <c r="C229" s="27" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="D229" s="25"/>
       <c r="E229" s="25" t="s">
@@ -10611,10 +10611,10 @@
         <v>274</v>
       </c>
       <c r="B269" s="26" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="C269" s="27" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="D269" s="25"/>
       <c r="E269" s="25" t="s">
@@ -10636,7 +10636,7 @@
         <v>275</v>
       </c>
       <c r="B270" s="26" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="C270" s="27" t="s">
         <v>528</v>
@@ -10686,10 +10686,10 @@
         <v>277</v>
       </c>
       <c r="B272" s="26" t="s">
+        <v>631</v>
+      </c>
+      <c r="C272" s="27" t="s">
         <v>633</v>
-      </c>
-      <c r="C272" s="27" t="s">
-        <v>635</v>
       </c>
       <c r="D272" s="25"/>
       <c r="E272" s="25" t="s">
@@ -11165,54 +11165,54 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A20:H52 A35:I289">
-    <cfRule type="expression" dxfId="13" priority="53">
+    <cfRule type="expression" dxfId="30" priority="53">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="54">
+    <cfRule type="expression" dxfId="29" priority="54">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="61">
+    <cfRule type="expression" dxfId="28" priority="61">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:H52 A35:I289">
-    <cfRule type="expression" dxfId="10" priority="7">
+    <cfRule type="expression" dxfId="27" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="8">
+    <cfRule type="expression" dxfId="26" priority="8">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="25" priority="9">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F289">
-    <cfRule type="expression" dxfId="7" priority="13">
+    <cfRule type="expression" dxfId="24" priority="13">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="14">
+    <cfRule type="expression" dxfId="23" priority="14">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:I52">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="22" priority="4">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="21" priority="5">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="20" priority="6">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:I52">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="19" priority="1">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="18" priority="2">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="17" priority="3">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>